<commit_message>
Updated pipeline to extract company name and MD&A boundary correctly
</commit_message>
<xml_diff>
--- a/mdna_extraction_project/output/mdna_extracted.xlsx
+++ b/mdna_extraction_project/output/mdna_extracted.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,25 +456,35 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>mdna_start_page</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>mdna_end_page</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>mdna_text</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>mdna_word_count</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>word_count</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>narrative_density</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>keyword_hits</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>quality_passed</t>
         </is>
@@ -488,8 +498,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>You are requested to take the above mentioned information on your records.
-For Alchemist Limited</t>
+          <t>ALCHEMIST LTD</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -503,6 +512,16 @@
         </is>
       </c>
       <c r="E2" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>V.
 INDEBTEDNESS - Indebtedness of the Company including interest outstanding/accrued but not due for payment.
@@ -1151,19 +1170,25 @@
 To look into the reasons for substantial defaults in the payment to the de</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>37325</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.7704144797642505</v>
-      </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>risk management, segment performance</t>
-        </is>
-      </c>
-      <c r="I2" t="b">
-        <v>0</v>
+          <t>37325</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0.7704144797642505</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>['risk management', 'segment performance']</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -1174,12 +1199,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Bankers
-Punjab National Bank
-Bank Of india
-HDFC Bank
-Registrar &amp; Share Transfers Agent
-Link Intime India Private Limited</t>
+          <t>ALCHEMIST LIMITED</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1193,6 +1213,16 @@
         </is>
       </c>
       <c r="E3" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>Annexure VI
 MANAGEMENT DISCUSSION AND ANALYSIS REPORT
@@ -1364,15 +1394,25 @@
 Time taken by executives to overcome from various new rules and regulations.</t>
         </is>
       </c>
-      <c r="F3" t="n">
-        <v>2740</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.8166772756206238</v>
-      </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="b">
-        <v>0</v>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2740</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>0.8166772756206238</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -1381,7 +1421,11 @@
           <t>ALok</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ALOK</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>5210700315.pdf</t>
@@ -1389,6 +1433,16 @@
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>PRIMED
 TO UNLOCK VALUE
@@ -2504,15 +2558,25 @@
 Plan period wit</t>
         </is>
       </c>
-      <c r="F4" t="n">
-        <v>16737</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.7509858872985687</v>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="b">
-        <v>0</v>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>16737</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>0.7509858872985687</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -2521,7 +2585,11 @@
           <t>ALok</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ALOK</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>5210700316.pdf</t>
@@ -2533,6 +2601,16 @@
         </is>
       </c>
       <c r="E5" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>Innovative Textile Solutions 43
 Form No. MR-3
@@ -3190,15 +3268,25 @@
 US$ 90 bn from the existing US$ 25 bn growing at</t>
         </is>
       </c>
-      <c r="F5" t="n">
-        <v>11815</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.755314143963047</v>
-      </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="b">
-        <v>0</v>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>11815</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>0.755314143963047</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -3207,7 +3295,11 @@
           <t>ALok</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ALOK</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>5210700317.pdf</t>
@@ -3219,6 +3311,16 @@
         </is>
       </c>
       <c r="E6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>As mentioned earlier, the overall performance of
 Alok industries in recent past has been impacted by
@@ -3269,15 +3371,25 @@
 Chairman</t>
         </is>
       </c>
-      <c r="F6" t="n">
-        <v>368</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.8202542744410346</v>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="b">
-        <v>0</v>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>368</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0.8202542744410346</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -3286,7 +3398,11 @@
           <t>ALok</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ALOK</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>5210700318.pdf</t>
@@ -3298,6 +3414,16 @@
         </is>
       </c>
       <c r="E7" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>(vi)
 The following laws are applicable to the Company :-
@@ -4159,19 +4285,25 @@
 (previous</t>
         </is>
       </c>
-      <c r="F7" t="n">
-        <v>9254</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.7307276690049268</v>
-      </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>risk management, global economy</t>
-        </is>
-      </c>
-      <c r="I7" t="b">
-        <v>0</v>
+          <t>9254</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0.7307276690049268</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>['risk management', 'global economy']</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -4196,6 +4328,16 @@
         </is>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>DIRECTORS’ REPORT
 Your Directors have great pleasure in presenting the 23rd Annual Report together with Audited Statements of Accounts of the Company for
@@ -4604,19 +4746,25 @@
 (g) Minutes of the Board meetings, Annu</t>
         </is>
       </c>
-      <c r="F8" t="n">
-        <v>5952</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.7747705665769082</v>
-      </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>risk management, future outlook</t>
-        </is>
-      </c>
-      <c r="I8" t="b">
-        <v>0</v>
+          <t>5952</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>0.7747705665769082</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>['risk management', 'future outlook']</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -4627,7 +4775,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>JM Financial Asset Reconstruction Company Pvt. Ltd.</t>
+          <t>AMIT SPINNING INDUSTRIES LIMITED</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -4642,7 +4790,272 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>SUBSIDIARY COMPANIES, JOINT VENTURES AND ASSOCIATE COMPANIES
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>N O T I C E
+Notice is hereby given that the 24th Annual General Meeting of the Members of Amit Spinning Industries Limited will be held
+on Tuesday the 27th day of September, 2016 at 12:00 Noon at Bipin Chandra Pal Memorial Bhavan, A-81, Chittaranjan
+Park, New Delhi 110019 to transact the following business:
+ORDINARY BUSINESS :
+1.
+To consider and adopt the Audited Financial Statements of the Company for the financial year ended 31st March, 2016,
+and the reports of the Board of Directors and Auditors thereon.
+2.
+To appoint a Director in place of Mr. Ranjan Mangtani (DIN: 00678341) who retires by rotation and being eligible, offers
+himself for re-appointment.
+3.
+To ratify the appointment of the Statutory Auditors of the Company for the year financial year 2016-17 and to fix their
+remuneration.
+SPECIAL BUSINESS:
+4. To consider and, if thought fit, to pass, with or without modifications the following resolution as an Ordinary Resolution:
+“RESOLVED THAT pursuant to the provisions of sections 149, 150, 152 and other applicable provisions and Schedule IV,
+of the Companies Act, 2013 read with the Companies (Appointment and Qualification of Directors) Rules, 2014, as may be
+amended from time to time, and SEBI (Listing Obligations and Disclosure Requirements) Regulations 2015, as may be
+amended, superseded or replaced from time to time, Mrs. Shivani Gupta (DIN 07547509), who was appointed as an
+Additional Director by the Board of Directors of the Company pursuant to section 161(1) of the Companies Act, 2013 and
+Article 85 of the Articles of Association and who holds office only upto the date of this Annual General Meeting and has
+submitted a declaration that she meets the criteria for independence as provided in section 149(6) of the Act and is eligible
+for appointment and in respect of whom the Company has received a notice in writing from a Member proposing her
+candidature for the office of Director, be and is hereby appointed as an Independent Non Executive Woman Director of the
+Company, for five consecutive years with effect from 30th June 2016 and whose office shall not be liable to retirement by
+rotation".
+"RESOLVED FURTHER THAT the Board of Directors of the Company be and is hereby authorized to do all such acts,
+matters, deeds and things as may be necessary, proper or expedient to give effect to the above resolution.”
+5.
+To consider and, if thought fit, to pass with or without modifications the following resolution as an Ordinary Resolution:
+“RESOLVED THAT pursuant to the provisions of Sections 196, 197, 203 and other applicable provisions of the
+Companies Act, 2013 and the Companies (Appointment and Remuneration of Managerial Personnel) Rules, 2014, read
+with Schedule V of the Companies Act, 2013, including any statutory modification(s) or re-enactment(s) thereof, and other
+requisite approvals as may be necessitated from time to time, the consent of the Company be and is hereby accorded for
+seeking Shareholders approval for appointment and fixation of remuneration to Mr. I D Desai as Manager to the Company
+for a period of three years w.e.f. 1st September, 2016, as per the terms and conditions set out in the explanatory statement
+annexed to the Notice convening this meeting with liberty to alter and vary the same upto 15% increase per annum on his
+remuneration, subject to maximum limits specified under Schedule V of the Companies Act, 2013 or any other statutory
+modification(s) or re-enactment thereof or in accordance with the approval of Shareholders of the Company.”
+"RESOLVED FURTHER THAT the Board of Directors of the Company be and is hereby authorized to do all such acts,
+matters, deeds and things as may be necessary, proper or expedient to give effect to the above resolution.”
+6.
+To consider and, if thought fit, to pass with or without modifications the following resolution as an Ordinary Resolution:
+“RESOLVED THAT pursuant to section 20 and other applicable provisions, if any, of the Companies Act, 2013 and
+relevant Rules prescribed thereunder, upon receipt of a request from a member for delivery of any document through a
+particular mode an amount of Rs.50/- (Rupees Fifty Only) for each such document, over and above reimbursement of
+actual expenses incurred by the Company, be levied as and by way of fees for sending the document to him in the desired
+particular mode.
+FURTHER RESOLVED THAT the estimated fees for delivery of the document shall be paid by the member in advance to
+the Company, before dispatch of such document.
+RESOLVED FURTHER THAT for the purpose of giving effect to this resolution, the Compliance Officer of the Company be
+and is hereby authorized to do all such acts, deeds, matters and things as he may in his absolute discretion deem
+necessary, proper, desirable or expedient and to settle any question, difficulty, or doubt that may arise in respect of the
+matter aforesaid, including determination of the estimated fees for delivery of the document to be paid in advance.”
+By Order of the Board
+For AMIT SPINNING INDUSTRIES LIMITED
+Place: New Delhi
+Sd/-
+Date : August 09, 2016
+Director
+NOTES:
+A.
+Explanatory Statement setting out all material facts regarding Special Business contained in Item Nos. 4 to 6 as required
+under Section 102 (1) of the Companies Act, 2013, is annexed hereto.
+B.
+A MEMBER ENTITLED TO ATTEND AND VOTE IS ENTITLED TO APPOINT A PROXY TO ATTEND AND VOTE
+INSTEAD OF HIMSELF/HERSELF AND THE PROXY NEED NOT BE A MEMBER OF THE COMPANY. PROXY
+SHOULD BE DEPOSITED AT THE REGISTERED OFFICE OF THE COMPANY ATLEAST 48 HOURS BEFORE THE
+COMMENCEMENT OF THE MEETING.
+C.
+A person can act as a proxy on behalf of members not exceeding fifty and holding in the aggregate not more than ten
+percent of the total share capital of the Company carrying voting rights. A member holding more than ten percent of the
+total share capital of the Company carrying voting rights may appoint a single person as proxy and such person shall not
+act as proxy for any other person or shareholder.
+D.
+The Register of Members and Share Transfer Books of the Company will be closed from Friday, the 23th day of
+September, 2016 to Tuesday the 27th day of September, 2016 (both days inclusive) for the purpose of this Annual
+General Meeting.
+E.
+All documents referred to in the Notice and accompanying explanatory statement are open for inspection at the
+Registered Office of the Company on all the working days of the Company between 10.00 A.M. to 1.00 P.M. upto the date
+of Annual General Meeting and also at the meeting.
+F.
+Members are requested to intimate the change, if any, in their registered address immediately.
+G. Members/Proxies should bring the attendance slips duly filled in and signed for attending the meeting.
+H.
+It will be appreciated that queries, if any, on accounts and operations of the Company are sent to the Registered Office of
+the company ten days in advance of the meeting so that the information may be made readily available.
+I.
+As per provisions of the Companies Act, facility of nomination is available to the members in respect of the shares held by
+them.
+J.
+For any query on the Depository System, members may contact any depository participant or the Share Department at the
+Registered Office of the Company.
+K.
+In terms of SEBI (Listing Obligations and Disclosure Requirements) Regulations, 2015, a brief resume of directors who
+are proposed to be appointed/re-appointed at this meeting is provided in Corporate Governance Report, forming part of
+the Annual Report.
+L.
+Securities and Exchange Board of India (SEBI) has made it mandatory for the transferees to furnish copy of PAN card to
+the Company/RTA for registration of shares held in Physical Form.
+M. Members are requested to send queries, if any, at E-mail ID secretarial@clcindia.com which is being used exclusively for
+the purpose of redressing the complaint(s) of the investors.
+N.
+VOTING THROUGH ELECTRONIC MEANS
+In accordance with provisions of section 108 of the Companies Act, 2013 read with Rule 20 of the Companies
+(Management and Administration) Rules, 2014 the business may be transacted through electronic voting system and the
+Company intends to provide facility for voting by electronic means ("e-voting") to its members. The Company has engaged
+the services of Central Depository Services (India) Limited (CDSL) to provide e-voting facilities and for security and
+enabling the members to cast their Vote in a secure manner. However, the Company has not paid the Annual Custodian
+Fee to the CDSL due the financial difficulties, the CDSL has blocked the benpos and not provided the shareholders list,
+and the Company is not in a position to conduct the e-voting process for the said meeting. Company has requested and
+assured the CDSL that the dues will be cleared once the rehabilitation scheme approved by the concerned authority
+inspite of our request, CDSL has not provided the benpos.
+ANNEXURE TO THE NOTICE
+EXPLANATORY STATEMENT PURSUANT TO SECTION 102(1) OF THE COMPANIES ACT, 2013
+ITEM NO. 4
+The Board of Directors had appointed Mrs. Shivani Gupta as an Additional Director of the Company on 30th June, 2016 under
+category of Independent Women Director.
+In terms of Section 161(1) of the Companies Act, 2013, Mrs. Shivani Gupta holds office upto the date of the ensuing Annual
+General Meeting. In this regard, the Company has received a notice in writing from a member alongwith deposit of requisite
+amount required under Section 160 of the Companies Act, 2013, proposing her candidature for the office of Independent
+Woman Director of the Company.
+In terms of the provisions of Section 149 of the Companies Act, 2013, an Independent Director shall hold office for a term up to
+five consecutive years on the Board of a company and is not liable to retire by rotation. Mrs. Shivani Gupta has given a
+declaration to the Board that she meets the criteria of independence as provided under Section 149 (6) of the Act.
+In compliance with the provisions of Section 149 read with Schedule IV of the Act, the appointment of Mrs. Shivani Gupta as
+Independent Women Director is now being placed before the Members in General Meeting for their approval.
+None of the Directors and/or Key Managerial Personnel of the Company and/or their relatives, except Mrs. Shivani Gupta is
+concerned or interested in the resolution set out in Item No. 4.
+Your Directors recommend the ordinary resolution set out at Item No. 4 of the Notice for your approval.
+ITEM NO. 5:
+Since the Managing Director Mr. I B Maner's term is expiring on 31st August, 2016 and keeping in view of financial difficulties,
+the Company cannot afford the remuneration payable to Managing Director and the Nomination and Remuneration
+Committee and Board of Directors at their meeting held on 9th August, 2016 have proposed to appoint Mr. Ishwar Dhondiba
+Desai as Manager to the Company w.e.f 1st September, 2016 as per the remuneration mutually agreed upon the Board and
+Mr. Desai.
+Mr. Desai aged about 58 years is a Post Graduate and having 30 years of rich experience in Human Resources and related
+matters and has been working with the Company for the past many years.
+As per the applicable provision read with Schedule V of the Companies Act, 2013, Company is not required to obtain the
+Central Government approval as the remuneration payable to Mr. I.D. Desai is within the limits prescribed under the said Act.
+OVERALL REMUNERATION
+Subject to the provisions of Section 196, 197 &amp; 203 read with Schedule V and other applicable provisions, if any, of the
+Companies Act, 2013 and the Companies (Appointment and Remuneration of Managerial Personnel) Rules 2014, the
+remuneration payable to a Manager in a financial year shall not exceed 5% of the net profit of the company computed in the
+manner laid down in section 198 except that the remuneration of the Directors shall not be deducted from the gross profits.
+Within the aforesaid ceiling, remuneration payable to Mr. I.D. Desai shall be as follows:
+I.
+Tenure of Remuneration
+1st September, 2016 to 31st August, 2019
+II.
+Remuneration
+Rs. 54,256/- including perquisites for aforesaid period subject to overall increase in
+remuneration shall be decided by the Chairman of the Company as per the relevant
+provisions on yearly basis and excluding the EPF, Gratuity/Superannuation fund and
+applicable incentives as mentioned in the Section 197 read with Schedule V of the
+Companies Act, 2013.
+III. Other terms of Appointment :
+a)
+No sitting fees shall be paid to them for attending meetings of Board of Directors/ Committee of the Board.
+b)
+Reimbursement of all entertainment, travelling, hotel and other expenses actually incurred by them in connection with
+the business of the Company.
+c)
+Normal annual Increment if any shall be decided by the Chairman of the Company as per the relevant provisions on
+yearly basis.
+The draft of Agreement to be entered into between the Company and Mr. I.D. Desai for appointment and remuneration is
+available for inspection by the members at the Registered Office of the Company during the business hours on any working
+day. The explanatory statement may also be regarded as a disclosure under SEBI (LODR) Regulations.
+None of the Directors and/or Key Managerial Personnel of the Company and/or their relatives, except Mr. I D Desai is
+concerned or interested in the resolution set out in Item No. 5.
+Your Directors recommend the ordinary resolutions set out at Item No. 5 of the Notice for your approval.
+ITEM NO. 6
+This is to inform to the members that pursuant to Section 20 of the Companies Act, 2013 and applicable provisions of the said Act,
+the company is required to serve a document to any member by sending it by Post or by Registered post or by Speed post or by
+Courier or by delivering at his office or address or by such electronic or other mode as may be prescribed by him from time to time.
+It is further informed that a member can request for delivery of any document to him through a particular mode for which he shall pay
+such fees as may be determined by the company in its Annual General Meeting. Therefore, to enable the members to avail of this
+facility, it is necessary for the Company to determine the fees to be charged for delivery of a document in a particular mode, as
+mentioned in the resolution. Since the Companies Act, 2013 requires the fees to be determined in the Annual General Meeting,
+None of the Directors and/or Key Managerial Personnel of the Company and their relatives is concerned or interested, financially or
+otherwise, in the resolution set out at Item No.6 of the accompanying Notice.
+Your Directors, accordingly, recommend this Ordinary Resolution at item no. 6 of the accompanying notice, for the approval of the
+members of the Company.
+BOARD'S REPORT
+Dear Members,
+Your Directors have great pleasure in presenting the 24th Annual Report together with Audited Statements of Accounts of the Company
+for the year ended March 31, 2016.
+Financial Results
+The summarized financial results for the year ended March 31, 2016 as compared to the previous year are as follows:
+(` in Lakhs)
+2015-2016
+2014-2015
+Revenue from Operation
+38.98
+3205.52
+Other Income
+1.63
+4.06
+Profit before depreciation, interest finance charges and tax (PBDIT)
+(847.18)
+(842.59)
+Less: Interest and Finance Charges
+309.38
+347.29
+Less: Depreciation
+346.61
+343.59
+Profit/(Loss) before Tax (PBT)
+(1503.17)
+(1533.46)
+Less : Tax Expense/Deferred Tax
+878.25
+Profit/(Loss) after Tax (PAT)
+(1503.17)
+(2411.71)
+FINANCIAL ANALYSIS AND PERFORMANCE REVIEW
+During the financial year 2015-16 under review, your company could not utilize its capacities due to financial constraints/shortage of
+working capital and the unit of the company located at Kolhapur remained inoperative accordingly the revenue from operations
+decreased to Rs. 38.98 lakhs as compared to Rs. 3,205.52 lakhs in the previous year.
+Further, over the period the company has eroded its net worth completely and it has been declared as a Sick Company under Sick
+Industrial Companies (Special Provisions) Act'1985 by the Board for Industrial and Financial Restructuring (BIFR) vide its order dated
+MANAGEMENT DISCUSSION AND ANALYSIS REPORT
+India’s Textiles Sector is one of the oldest Industry in Indian economy dating back several centuries. Even today, textiles sector is one of
+the largest contributor to India’s exports accounting for approximately 11% of total exports. The Textile Industry is also labor intensive
+and is one of the largest employers. The industry realised export earnings worth US$ 41.4 billion and a growth of 5.4 per cent.
+The textile industry has two broad segments. First, the unorganised sector consists of handloom, handicrafts and sericulture, which are
+operated on a small scale and through traditional tools and methods. The second is the organized sector consisting of Spinning,
+Apparel and Garment segment which apply modern machinery and technology.
+Amit Spinning is producing only Cotton Yarn with a capacity of 30672 spindles. However, during the period under review, the operations
+of Amit Spinning were badly affected due to shortage of Working Capital and non approval of Rehabilitation Plan by BIFR.
+Due to these constraints the Company operations have been suspended since 11th August, 2015 resulting in revenue from
+operations decreasing to Rs. 38.98 Lakhs as compared to Rs. 32.05 Crores during 2014-15.
+MANAGEMENT PERCEPTION ON OPPORTUNITIES, RISKS, CONCERN &amp; OUTLOOK
+The Low per-capita domestic consumption of textile indicates potential of growth in the textile industry. The Indian government has
+come up with a number of export promotion policies for the textiles sector. A new National Textiles Policy is expected to be announced
+soon Further, the Government has proposed the establishment of Centres of Excellence for training the workforce in the textile sector
+and also to establish institutes under the public-private partnership (PPP) model to encourage private sector participation in the
+development of the industry.
+Further, with focus on Make in India, the Indian Textile industry is expected to become resilient and robust through various support
+measures likely to be announced by the government. The future outlook for the Indian Textile Industry looks promising, buoyed by both
+strong domestic consumption and increase in export turnover.
+The major factors hindering progress of the textiles industry are Increase in the power costs, higher transaction costs, high cost of
+labour and general increase in input costs, thus the industry has to concentrate on cost reduction exercises and improvement in
+efficiency. With conscious and focused efforts and strategies built around optimum product mix, operational efficiencies and customer
+satisfaction the management is confident of a turnaround of the company in near future.
+With the awaited / impending approval of rehabilitation scheme of the company by BIFR and with the continued support and co-
+operation of company’s bankers, management believes that your Company would again resume production, optimally utilize
+capacities, and generate increasing sales volumes, margins in due course.
+SEGMENT-WISE PERFORMANCE
+Amit Spinning Industries Ltd. (ASIL) being a cotton yarn manufacturer has only one business segment. On the basis of geographical
+categorization of market, ASIL identified two segments i.e. exports and domestic.
+During the year under review, Company has not manufactured yarn as against 1281.64 MT produced by the company in the previous
+year.
+SUBSIDIARY COMPANIES, JOINT VENTURES AND ASSOCIATE COMPANIES
 As there are no subsidiaries/associates/joint ventures of the Company, the provisions contained in Companies Act, 2013/ SEBI
 (LODR) Regulations relating to subsidiaries are not applicable.
 DIVIDEND
@@ -4786,128 +5199,1004 @@
 8 of the Companies (Accounts) Rules, 2014 is set out in the Annexure – 4 to this Report.
 PARTICULARS OF EMPLOYEES
 The statement containing particulars of employees as required under section 197(12) of the Act read with Rule 5(2) &amp; 5(3) of the
-Companies (Appointment and Remuneration of Managerial Personnel) Rules, 2014 as amended, shall be made available to any
-shareholder on a specific request made by him in writing on or before 27th September, 2016.
+Companies (Appointment and Remuneration of Managerial Personnel) Rules, 2014</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>8922</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>0.7677311237314961</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>['risk management', 'future outlook']</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Amit_spinning</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>AMIT SPINNING INDUSTRIES LIMITED</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>5210760317.pdf</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2016-17</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>BOARD OF DIRECTORS
+REGISTERED &amp; CORPORATE OFFICE
+S P Setia
+(Non-Executive / Independent Chairman)
+A-60, Okhla Industrial Area,
+I. D. Desai
+(Manager)
+Phase - II, New Delhi - 110020
+Shivani Gupta
+(Non-Executive / Independent Woman Director)
+K Sankaramani
+(Non-Executive Director)
+Vijay Bhan Singh
+(Non-Executive Director)
+REGISTRAR &amp; TRANSFER AGENTS
+M/s. RCMC Share Registry Pvt. Ltd.
+B-25/1, Okhla Industrial Area, Phase-II,
+Near Rana Motor, New Delhi - 110020
+PLANT
+Gat No. 47 &amp; 48, Sangavade Village
+Kolhapur - Hupari Road
+Taluka Karveer
+Dist. Kolhapur 416 202
+MAHARASHTRA
+BANKERS / ARC
+AXIS Bank Limited
+JM Financial Asset Reconstruction
+Company Pvt. Ltd.
+AUDITORS
+Sunil Jain &amp; Co.
+Chartered Accountants
+New Delhi
+AUDIT COMMITTEE
+S P Setia (Chairman)
+K. Sankaramani
+Shivani Gupta
+NOMINATION AND REMUNERATION COMMITTEE
+S P Setia (Chairman)
+K. Sankaramani
+Shivani Gupta
+STAKEHOLDERS RELALTIONSHIP COMMITTEE
+S P Setia (Chairman)
+K. Sankaramani
+Shivani Gupta
+INDEX
+Page No.
+Notice
+Board’s Report Including
+Management Discussions &amp;
+Analysis Report
+Annexures to Boards’ Report
+Corporate Governance
+Auditor’s Report
+Balance Sheet
+Statement of Profit &amp; Loss
+Cash Flow Statement
+Notes
+25th AGM
+Date
+September 25, 2017 Time 11:30 A.M.
+Venue
+Bipin Chandra Pal Memorial Bhavan, A-81, Chittaranjan Park, New Delhi - 110 019
+Book Closure :
+From Thursday September 21, 2017 to Monday, September 25, 2017 (both days inclusive).
+Company’s shares are listed on BSE Ltd. and National Stock Exchange of India Ltd.
+N O T I C E
+NOTICE is hereby given that the 25th Annual General Meeting of the Members of Amit Spinning Industries Limited will
+be held on Monday the 25th day of September, 2017 at 11.30 A.M at Bipin Chandra Pal Memorial Bhavan, A-81,
+Chittaranjan Park, New Delhi 110019 to transact the following business:
+ORDINARY BUSINESS:
+1.
+To consider and adopt the Audited Financial Statements of the Company for the financial year ended 31st March,
+2017 including Balance Sheet of the Company as at 31st March, 2017, Statement of Profit &amp; Loss for the year ended
+on that date and the Reports of the Board of Directors' and Auditors' thereon.
+2.
+To ratify appointment of the Statutory Auditors of the Company for the financial year 2017-18 and to fix their remuneration.
+SPECIAL BUSINESS:
+3.
+To consider and, if thought fit, to pass with or without modifications the following resolution as an Ordinary Resolution:
+"RESOLVED THAT pursuant to the provisions of sections 149, 152 and other applicable provisions, if any, of the
+Companies Act, 2013 read with Companies (Appointment and Qualification of Directors) Rules, 2014 and SEBI
+(Listing Obligation and Disclosure Requirements) Regulations 2015 (including any statutory modification(s) or re-
+enactment thereof, for the time being in force) , Mr. Vijay Bhan Singh (DIN 07764296), who was appointed as an
+Additional Director by the Board of Directors of the Company pursuant to section 161(1) of the Companies Act, 2013
+and Article 85 of the Article of Association of the company and who holds office up to the date of this Annual General
+Meeting and in respect of whom the Company has received a notice in writing from a member alongwith the requisite
+fee proposing his candidature for the office of director, be and is hereby appointed as Non Executive Director of the
+Company and who shall be liable to retire by rotation".
+For &amp; on behalf of the Board
+Sd/-
+Director
+(Signed under the authority of Parveen Bansal, who has been appointed as Interim Resolution Professional by
+order of Principal Bench, National Company Law Tribunal dated August 1, 2017 under the provisions of
+Insolvency and Bankruptcy Code, 2016)
+Place : New Delhi
+Date : 17th August, 2017
+NOTES:
+A.
+Explanatory Statement setting out all material facts regarding Special Business contained in Item Nos. 3 as required
+under Section 102 (1) of the Companies Act, 2013, is annexed hereto.
+B.
+A MEMBER ENTITLED TO ATTEND AND VOTE IS ENTITLED TO APPOINT A PROXY TO ATTEND AND VOTE
+INSTEAD OF HIMSELF/HERSELF AND THE PROXY NEED NOT BE A MEMBER OF THE COMPANY. PROXY
+SHOULD BE DEPOSITED AT THE REGISTERED OFFICE OF THE COMPANY ATLEAST 48 HOURS BEFORE
+THE COMMENCEMENT OF THE MEETING.
+C. A person can act as a proxy on behalf of members not exceeding fifty and holding in the aggregate not more than ten
+percent of the total share capital of the Company carrying voting rights. A member holding more than ten percent of
+the total share capital of the Company carrying voting rights may appoint a single person as proxy and such person
+shall not act as proxy for any other person or shareholder.
+D. The Register of Members and Share Transfer Books of the Company will be closed from Thursday, the 21st day of
+September, 2017 to Monday, the 25th day of September, 2017 (both days inclusive) for the purpose of this Annual
+General Meeting.
+E.
+All documents referred in the Notice and accompanying explanatory statement are open for inspection at the Registered
+Office of the Company on all working days of the Company between 10.00 A.M. to 1.00 P.M. upto the date of Annual
+General Meeting and also at the meeting.
+F.
+Members are requested to intimate the change, if any, in their registered address immediately.
+G.
+Members/Proxies should bring the attendance slips duly filled in and signed for attending the meeting.
+H. It will be appreciated that queries, if any, on accounts and operations of the Company are sent to the Registered Office
+of the company ten days in advance of the meeting so that the information may be made readily available.
+I.
+As per provisions of the Companies Act, facility of nomination is available to the members in respect of the shares
+held by them.
+J.
+For any query on the Depository System, members may contact any depository participant or the Share Department
+at the Registered Office of the Company.
+K.
+In terms of SEBI (Listing Obligation and Disclosure Requirements) Regulations, 2015, a brief resume of directors who
+are proposed to be appointed at this meeting is provided in Corporate Governance Report, forming part of the Annual
+ANNEXURE TO THE NOTICE
+EXPLANATORY STATEMENT PURSUANT TO SECTION 102(1) OF THE COMPANIES ACT, 2013
+ITEM NO. 3:
+Mr. Vijay Bhan Singh was appointed as an Additional Director on the position of Non-Executive Director of the Company
+on 27th March, 2017 by the Board of Directors of the Company and holds office upto the date of this Annual General
+Meeting. Mr. Singh (52 years) is Commerce Graduate and having rich experience in Accounts, finance and related
+matters.
+The Company has received a notice in terms of Section 160 of the Companies Act, 2013 alongwith the amount of requisite
+deposit from a member signifying his intention to propose the appointment of Mr. Vijay Bhan SIngh as a Director of the
+Company.
+As required under Section 152 of the Companies Act, 2013, the Company has received a declaration from Mr. Vijay Bhan
+Singh that he is not disqualified from being appointed as a Director in terms of Section 164 of the Act and has given his
+consent to act as a Director.
+Brief resume of Mr. Vijay Bhan Singh, nature of his expertise in specific functional areas are provided in the Corporate
+governance Report forming part of the Annual Report.
+None of the Directors and/or Key Managerial Personnel of the Company and/or their relatives, except Mr. Vijay Bhan
+Singh is concerned or interested in the resolution set out in Item No. 3.
+Board/ Interim Resolution Professional recommends the resolution in relation to appointment of Mr. Vijay Bhan Singh as
+a Director, for the approval by the shareholders of the Company.
+For &amp; on behalf of the Board
+Sd/-
+Director
+(Signed under the authority of Parveen Bansal, who has been appointed as Interim Resolution Professional by
+order of Principal Bench, National Company Law Tribunal dated August 1, 2017 under the provisions of
+Insolvency and Bankruptcy Code, 2016)
+Place : New Delhi
+Date : 17th August, 2017
+Report.
+L.
+Securities and Exchange Board of India (SEBI) made it mandatory for the transferees to furnish copy of PAN card to
+the Company/RTA for registration of shares held in Physical Form.
+M. Members are requested to send queries, if any, at E-mail ID secretarial@clcindia.com which is being used exclusively
+for the purpose of redressing the complaint(s) of the investors.
+N. VOTING THROUGH ELECTRONIC MEANS
+In accordance with provisions of section 108 of the Companies Act, 2013 read with Rule 20 of the Companies
+(Management and Administration) Rules, 2014 the business may be transacted through electronic voting system and
+the Company intends to provide facility for voting by electronic means ("e-voting") to its members. The Company has
+engaged the services of Central Depository Services (India) Limited (CDSL) to provide e-voting facilities and for
+security and enabling the members to cast their vote in a secure manner. However, the company has not paid the
+Annual Custodian Fee to the CDSL due to financial difficulties, the CDSL/NSDL have blocked the benpos and not
+provided the shareholders list, and the company is not in a position to conduct the e-voting process for the said
+meeting. Company has requested and assured the CDSL that the dues will be cleared, inspite of our request, CDSL
+has not provided the benpos.
+BOARD'S REPORT
+Dear Members,
+Your Directors have great pleasure in presenting the 25th Annual Report together with Audited Statements of Accounts of
+the Company for the year ended March 31, 2017.
+FINANCIAL RESULTS:
+The summarized financial results for the year ended March 31, 2017 as compared to the previous year are as follows:
+( in Lakhs)
+FINANCIAL ANALYSIS AND PERFORMANCE REVIEW
+During the financial year 2016-17 under review, due to financial constraints and shortage of working capital the Company
+operations have remained suspended since 11th August, 2015 resulting in revenue from operations decreased in the
+current financial year ended 31st March, 2017 to Rs. 15.85 Lakhs as compared to Rs. 38.98 Lakhs during previous year
+ended 31st March, 2016.
+Further, the manufacturing unit situated at Kolhapur, Maharashtra stand closed with effect from 1st July, 2017 in accordance
+with applicable legal provisions.
+The Company was declared as a Sick Company under Section 3(1)(o) of SICA 1985., SICA has been repealed w.e.f. 1st
+December, 2016, and such companies were allowed to approach (NCLT) within 180 days. Accordingly, the Company has
+filed its petition before NCLT for resolution of default of payments to banks and other creditors and approval of Resolution
+Plan and NCLT has pronounced the commencement of a corporate insolvency resolution process, effective August 1,
+2017 and Mr. Parveen Bansal, has been appointed as Interim Resolution Professional in accordance with applicable
+regulations under Insolvency and Bankruptcy Code, 2016.
+MANAGEMENT DISCUSSION AND ANALYSIS REPORT
+The Indian textiles industry is one of the oldest industries in India having evolved impressively from a domestic small scale
+industry to becoming a major employment and GDP contributor with a massive manufacturing base. It is also one of the
+largest and most important sectors of the Indian economy in terms of output, foreign exchange earnings thus contributing
+greatly to the exchequer. The Textile sector occupies a unique position as a self-reliant industry, with substantial value-
+addition at each stage of processing. It has vast potential for creation of employment opportunities in the agricultural,
+industrial, organized &amp; decentralized sectors and 5.8 million cotton farmers, 40 to 50 million people engaged in textile
+related activities in rural and urban areas, particularly for un-educated, women &amp; unskilled labour. Thus, the growth and all
+round development of this sector has a direct bearing on the development of the economy.
+Amit Spinning has capacity to produce Cotton Yarn with 30672 spindles. During the period under review, the operations of
+Amit Spinning were badly affected due to shortage of Working Capital. Due to the financial constraints the Company
+operations have been suspended since 11th August, 2015 resulting in revenue from operations decreased in the current
+financial year ended 31st March, 2017 to Rs. 15.85 Lakhs as compared to Rs. 38.98 Lakhs during previous year ended
+31st March, 2016.
+As members of Amit Spinning are aware that the Company was declared as a Sick Company under Section 3(1)(o) of
+SICA 1985, from 1st December, 2016, SICA has been repealed and such companies were allowed to approach National
+Company Law Tribunal (NCLT) within 180 days. Accordingly, the Company has filed its petition before NCLT for resolution
+of its debts and approval of resolution plan
+In addition to the above, the manufacturing unit situated at Kolhapur, Maharashtra stand closed with effect from 1st July,
+2017 in accordance with applicable legal provisions due to shortage of working capital and closing of unit is a major jolt to
+the Company.
+However, with due strategic focus on Company by the management towards arrangement of funds through various
+options, Amit Spinning is confident to re-start its manufacturing unit in near future.
+MANAGEMENT PERCEPTION ON OPPORTUNITIES, RISKS, CONCERN &amp; OUTLOOK
+The Indian government has come up with the Revised Restructured Technology Up gradation Fund Scheme (RRTUFS),
+10% capital subsidy to the specified technical textile machinery, allowing 100% FDI in the Indian textiles sector under the
+automatic route may increase the profits in the coming years, the future of the Indian textile industry looks promising,
+Particulars
+2015-2016
+2016-2017
+Revenue from Operation
+15.85
+38.98
+Other Income
+0 .76
+1.63
+Profit before depreciation, interest finance charges and tax (PBDIT)
+(1023.75)
+(847.18)
+Less: Interest and Finance Charges
+1.86
+309.38
+Less: Depreciation
+296.82
+346.61
+Profit/(Loss) before Tax (PBT)
+(1322.43)
+(1503.17)
+Less : Tax Expense/Deferred Tax
+Profit/(Loss) after Tax (PAT)
+(1322.43)
+(1503.17)
+buoyed by both strong domestic consumption as well as export demand. With consumerism and disposable income on
+the rise, the retail sector has experienced a rapid growth in the past decade with the entry of several international players.
+Further, the Textile Ministry has also introduced a new textile policy to promote value additions which sets a target of
+doubling textile exports in next 10 years.
+The major factors hindering progress of the textiles industry are increase in the power costs, higher transaction costs, high
+cost of labour and general increase in input costs, thus the industry has to concentrate on cost reduction exercises and
+improvement in efficiency. Another key challenge presently is the Fiber/Raw Material cost, which is increasing abruptly
+and increase is not fully absorbed in the yarn prices and accordingly yarn spinners are hit the most in the entire textile
+chain.
+Due to fluctuating prices and uncertainties in the foreign exchange market, increase in power cost, introduction of GST
+and lack of adequate working capital, the EBITA levels may remain stagnant during the year.
+Further, to overcome the losses promptly in this challenging scenario, the Management is keeping a close watch on
+various threats/risks facing the company and taking all appropriate steps to restart of manufacturing unit.
+With much awaited / impending approval of rehabilitation scheme of the Company by NCLT and with the continued
+support and co-operation of company's bankers, management believes that your Company would again resume production,
+optimally utilize capacities, and generate increasing sales volumes, margins in due course and the management is
+confident of a turnaround of the company in near future.
+SEGMENT-WISE PERFORMANCE
+Amit Spinning Industries Ltd. (ASIL) being a cotton yarn manufacturer has only one business segment. On the basis of
+geographical categorization of market, ASIL identified two segments i.e. exports and domestic. During the year under
+review, Company has not manufactured yarn due to suspension of operations of manufacturing unit.
+SUBSIDIARY COMPANIES, JOINT VENTURES AND ASSOCIATE COMPANIES
+As there are no subsidiaries/ associates / joint ventures of the Company, the provisions contained in Companies Act,
+2013/SEBI (LODR) Regulations relating to subsidiaries are not applicable.
+DIVIDEND
+During the year under review, the Company has no distributable profits hence directors regret their inability to recommend
+any dividend for financial period 2016-17.
+TRANSFER OF RESERVES
+During the year, the Company has not transferred any amount to reserves.
+SHARE CAPITAL
+The Company's Authorized Share Capital as on 31st March, 2017 stands at Rs. 25,00,00,000/- and issued &amp; paid up
+capital as on 31st March, 2017 stands at Rs. 20,58,48,335/- divided into 4,11,69,667 fully paid up equity shares of Rs.5/-
+each. During the year, under review, the Company has not issued any share(s). Further the Company has not issued any
+share with differential Voting Rights/Sweat Equity shares/under Stock Option Scheme (ESOS) earlier and during the year.
+The Company has no scheme of provision of money for purchase of its own shares by employees or by trustees for the
+benefit of employees. Hence the details under rule 16 (4) of Companies (Share Capital and Debentures) Rules, 2014 are
+not required to be disclosed.
+DIRECTORS AND KEY MANAGERIAL PERSONNEL
+(a) Change in Directors and Key Managerial Personnel
+Mr. Vijay Bhan Singh has been appointed as an Additional Non-Executive Director on the Board of the Company with
+effect from 27th March, 2017.
+Mr. Ranjan Mangtani, Non-Executive Director has tendered his resignation w.e.f. closing hours of 10th November,
+2016. During the year, the term of I.B. Maner as Managing Director has expired on closing hours of 31st August, 2016
+and has resigned from directorship w.e.f. 10th November, 2016 keeping in view of financial difficulties of the Company,
+members of the Company have appointed Mr. I D Desai as Manager for a period of 3 years w.e.f. 1st September, 2016.
+Further, during the year, under review, Ms. Priya Lohani, Company Secretary has resigned w.e.f. 22nd June, 2016 and
+Company has appointed Mr. Deepanshu Arora as Compliance Officer to the Company w.e.f 9th August, 2016, he has
+also tendered his resignation and subsequently, Mr. Bharat Kapoor has been appointed as Compliance Officer of the
+Company w.e.f 31st December, 2016 in place of Mr. Deepanshu Arora.
+Mr. K. Sankaramani, Non Executive Director and Mr. Malpeddi Nagnath S, CFO have resigned w.e.f. 1st August, 2017.
+Brief resume of the Director(s) proposed to be appointed/re-appointed, nature of their expertise in specific functional
+areas and names of the companies in which they hold directorship and membership/chairmanships of the Board or its
+Committees, as stipulated under SEBI (LODR) Regulations entered into by the Company with stock exchanges in
+India, is provided in the Report of Corporate Governance forming part of the Annual Report.
+(b) Number of Meetings of the Board
+Five meetings of the Board were held during the year. The detailed information regarding meetings of the Board held
+during the year is mentioned in the Corporate Governance Report which forms part to this report.
+(c) Declaration by Independent Directors
+All Independent Directors have given declarations that they meet the criteria of independence as laid down under
+Section 149(6) of the Companies Act, 2013 and SEBI (LODR) Regulations.
+(d) Annual Evaluation by the Board
+Pursuant to the provisions of the Companies Act, 2013 and SEBI (LODR) Regulations, the Board has carried out an
+annual performance evaluation of its own performance, the directors individually as well as its Committees. The
+manner in which the evaluation has been carried out has been explained in the Corporate Governance Report.
+(e) Remuneration Policy
+The Board has, on the recommendation of the Nomination &amp; Remuneration Committee framed a policy for selection
+and appointment of Directors, Senior Management and their remuneration. The Remuneration Policy is enumerated
+in the Corporate Governance Report. During the year, neither the Managing Director nor the Whole-time Directors of
+the Company received any remuneration or commission from any of its subsidiaries.
+DIRECTORS' RESPONSIBILITY STATEMENT
+Pursuant to the requirement of Section 134(3) (c) of the Companies Act, 2013, with respect to Directors' Responsibility
+Statement, it is hereby confirmed that:
+(a) in the preparation of the annual accounts for the financial year ended 31st March, 2017, the applicable accounting
+standards had been followed along with proper explanation relating to material departures;
+(b) the directors had selected such accounting policies and applied them consistently and made judgments and
+estimates that are reasonable and prudent so as to give a true and fair view of the state of affairs of the company
+as at March 31, 2017 and of the profit and loss of the company for that period;
+(c) the directors had taken proper and sufficient care for the maintenance of adequate accounting records in accordance
+with the provisions of the Companies Act, 2013 for safeguarding the assets of the company and for preventing and
+detecting fraud and other irregularities;
+(d) the directors had prepared the annual accounts on a going concern basis; and
+(e) the directors had laid down internal financial controls to be followed by the company and that such internal
+financial controls are adequate and were operating effectively.
+(f) the directors had devised proper systems to ensure compliance with the provisions of all applicable laws and that
+such systems were adequate and operating effectively.
+RELATED PARTY TRANSACTIONS
+None of the transactions with related parties falls under the scope of section 188(1) of the Act. All related party transactions
+that were entered into during the financial year were on an arm's length basis and were in the ordinary course of business.
+There were no materially significant related parties transactions entered into by the Company with Holding Company/
+Promoters, Directors, Key Managerial Personnel or other designated persons which may have a potential conflict with the
+interest of the Company at large.
+Prior omnibus approval of the Audit Committee was obtained for Related Party Transactions for the year ended 31st
+March, 2017 and for transactions proposed to be entered into with related parties for the financial year 2017-18 were
+placed before the said committee and consent of the said committee was obtained.
+The policy on Related Party Transactions as approved by the Board has been uploaded on the Company's website
+www.spentex.net. None of the Directors has any pecuniary relationships or transactions vis-a-vis the Company. Since all
+related party transactions entered into by the Company were in ordinary course of business and were on an arm's length
+basis, form AOC - 2 is not applicable to the Company.
+MATERIAL CHANGES AND COMMITMENTS AFFECTING THE FINANCIAL POSITION BETWEEN THE DATE OF THE
+BOARD REPORT AND END OF FINANCIAL YEAR
+The operations of manufacturing unit situated at Kolhapur, Maharashtra remains closed with effect from 1st July, 2017
+after completion of applicable legal formalities.
+As the Company was declared as a Sick Company under Section 3(1)(o) of SICA 1985 and SICA has been repealed w.e.f
+1st December, 2016, accordingly, the Company had filed its petition before NCLT under Insolvency and Bankruptcy Code,
+2016 and NCLT has pronounced the order admitting the petition of the Company, and appointing Mr. Parveen Bansal, as
+an Interim Resolution Professional in accordance with applicable regulations under Insolvency and Bankruptcy Code,
+2016. With this, corporate insolvency resolution process, against the Company Commences w.e.f 1st August, 2017.
+SIGNIFICANT AND MATERIAL ORDERS PASSED BY THE REGULATORS OR COURTS.
+NCLT has, vide its order dated 1st August, 2017, admitted Company's petition under Insolvency and Bankruptcy Code,
+2016 and has appointed Interim Resolution Professional and with that Corporate Insolvency Resolution Process in respect
+of the Company under IBC, 2016, commences.
+AUDITORS AND AUDITORS REPORT
+(a) Statutory Auditors
+At the 22nd Annual General Meeting held on 11.09.2014, M/s Sunil Jain &amp; Co., Chartered Accountants, (Firm Registration
+No. 003855N) was appointed as Statutory Auditor of the Company to hold office till the conclusion of the 26th Annual
+General Meeting to be held in the Calendar Year 2018. In terms of the proviso to Section 139 of the Companies Act,
+2013, the appointment of the Auditors shall be placed for ratification at every Annual General Meeting. Therefore, the
+appointment of M/s. Sunil Jain &amp; Co., Chartered Accountants, as statutory auditors of the Company is placed for
+ratification by the shareholders. The Company has received a confirmation from M/s. Sunil Jain &amp; Co., Chartered
+Accountants to the effect that their appointment, if made, at the ensuing AGM would be in terms of Sections 139 and
+141 of the Companies Act, 2013 and rules made there under and that they are not disqualified for re-appointment.
+Further, the Statutory Auditors have submitted Auditors' Report on the accounts of the Company for the period ended
+Directors' view on Auditor's Observations
+Directors' response to the various observations of the auditors made in their report, have been explained wherever
+necessary through appropriate notes to accounts, however pertinent notes are reproduced hereunder in compliance with
+the relevant legal requirements and wherever required further explanation is furnished:
+Note No. 30 of the Financial Statement qualified by Auditors
+The Company has not charged interest amounting to Rs.6,98,32,251. Further the company has not charged penal interest
+and other charges, if any, in respect of delay in repayment of borrowings from banks to the statement of profit and loss
+account from the date of declaration of account as Non Performing Assets.
+The management is of the opinion that since the lenders have categorized their outstanding debts from the Company and
+stopped charging interest on their debt, the management has decided not to provide interest on such loans for the current
+year and also reversed interest provided earlier years from the date of NPA.
+Note No. 28 of the Financial Statement without qualifying, Auditors have drawn attention:
+The outstanding balances of parties under the head trade payables and loans &amp; advances and Banks and other deposite
+are subject to confirmation, reconciliation and consequential adjustments arising there from if any. The management,
+however, does not expect any material variations.
+Note No. 29 of the Financial Statement without qualifying, Auditors have drawn attention:
+As on March 31, 2017, the accumulated losses of the Company have far exceeded its net worth. In the opinion of the
+management, the Company's operations were in the earlier years affected by global business downturn which has resulted
+in reduction in demand, increase in input costs and shortage of working capital. Due to these factors, the Company had
+filed a reference with Board for Industrial and Financial Restructuring (BIFR) under section 15 of Sick Industrial Companies
+(Special Provisions) Act, 1985 for determination of sickness and measures to be adopted for rehabilitation. The BIFR, vide
+its order, dated 18.07.2012 declared the Company as sick under section 3(1)(o) of SICA, 1985 and appointed UCO Bank
+as Operating Agency (OA) under section 17(3) to prepare Rehabilitation Scheme for the Company. The Company's
+accounts have become Non Performing Assets (NPA) with all the dealing banks and the company is also in receipt of NPA
+cum recall notice. Pending approval of DRS by OA/ BIFR, SICA has been repealed w.e.f 1/12/2016, and 6 months window
+has been provided to the Company to approach to National Company Law Tribunal (NCLT), as per section 4(b) of the
+SICA repeal act read with Sec. 252 of the Insolvency and Bankruptcy Code, 2016 to initiate Corporate Resolution Process
+under the code. Company is in the process of moving NCLT for resolution of its liabilities. In the meanwhile, Axis Bank has
+initiated recovery proceedings before DRT against the Company, however the same is being contested by the company.
+The company has submitted restructuring proposal proposing various alternative to the banks which is currently under
+discussion. With strong management focus on strategic initiatives on cost rationalization, optimum product mix and
+efficient plant operations, the management believes that accumulated losses would reasonably be paired in due course.
+Thus, on the strength of management's plan of revival including reorganization of business, these financial statements are
+prepared on a going concern basis.
+As per management, the company has filed its petition before NCLT for resolution of its debts and approval of rehabilitation
+scheme and NCLT has pronounced the commencement of a corporate insolvency resolution process, against the Company
+w.e.f 1st August, 2017 in accordance with applicable regulations under Insolvency and Bankruptcy Code, 2016.
+Note No. 31 of the Financial Statement without qualifying, Auditors have drawn attention:
+The company has advanced an amount of Rs.27,77,23,608/- as Inter Corporate Deposit and Capital Advances without
+any repayment schedule and interest free. The management is however hopefull of recovering the same in full. Auditors
+have relied upon the assertions given by the management as to the recoverability of the said amounts.
+(b) Cost Auditor:
+The Company having been declared as a sick company under repealed SICA and having not produced any yarn in the
+year 2016-17, the Companies (Cost Records and Audit Rules), 2014 is not applicable to the Company.
+(c) Secretarial Auditor &amp; Audit Report:
+Pursuant to provisions of Section 204 of the Companies Act, 2013, the Company has appointed M/s. Loveneet Handa
+&amp; Associate, Practicing Company Secretary (having CP No. 10753 &amp; Membership No. F-9055) as Secretarial Auditor
+to carry out the secretarial audit for the financial year 2016-17. The Secretarial Audit Report for the financial year
+ended March 31, 2017 in Form MR-3 is annexed herewith as Annexure I to this Report in compliance with the provisions
+of Section 204 of the Companies Act, 2013.
+The qualifications/observations/remarks made by the Secretarial Auditors and management's view thereon are given
+in their Report attached hereto.
+(d) Internal Auditors
+During the year, Dr. Sunil Kumar Gupta is Internal Auditor of the Company pursuant to section 138 of the Companies
+Act, 2013 read with The Companies (Accounts) Rules, 2014. However he has tendered his resignation w.e.f. 25th
+July, 2017.
+INTERNAL CONTROL SYSTEMS AND ADEQUACY
+The Company has established adequate internal control systems, commensurate with its size and nature of business and
+such systems are periodically audited, verified and reviewed for their validity, considering the changing business scenario
+from time to time, the Audit Committee of the Board of Directors reviews the adequacy and effectiveness of internal
+control systems and suggests improvement for strengthening them.
+EXTRACT OF THE ANNUAL RETURN
+The details forming part of the extract of the Annual Return in form MGT 9 is annexed herewith as Annexure-2 to this
+Report.
+CONSERVATION OF ENERGY, TECHNOLOGY ABSORPTION AND FOREIGN EXCHANGE EARNINGS AND OUTGO.
+As there is no operation/production during the year under review, the information as required to be disclosed under
+Section 134(3)(m) of the Companies Act, 2013 read with Rule, 8 of the Companies (Accounts) Rules, 2014 is not applicable.
+PARTICULARS OF EMPLOYEES
+The statement containing particulars of employees as required under section 197(12) of the Act read with Rule 5(2) &amp; 5(3)
+of the companies (Appointment and Remuneration of Managerial Personnel) Rules, 2014 as amended, shall be made
+available to any shareholder on a specific request made by him in writing on or before 25th September, 2017.
 DEPOSITS
-The Company has not accepted or renewed any deposit during the year and there are no outstanding and/or overdue deposits as at
-31st March, 2016.
+The Company has not accepted or renewed any deposit during the year and there are no outstanding and/or overdue
+deposits as at 31st March, 2017.
 PARTICULARS OF LOANS, GUARANTEES OR INVESTMENTS
-Details of loans, Guarantees and Investments covered under the provision of Section 186 of the Companies Act, 2013 are given in the
-notes to the Financial Statements.
+Details of loans, Guarantees and Investments covered under the provision of Section 186 of the Companies Act, 2013 are
+given in the notes to the Financial Statements.
 RISK MANAGEMENT
-A Risk Management Committee has been constituted to oversee the risk management process in the Company as required under the
-Companies Act, 2013 and SEBI (LODR) Regulations. The details of the Committee and its terms of reference are set out in the
-Corporate Governance Report forming part of the Board's Report. The Risk Management Policy has also been hosted on the website
-of the company
+A Risk Management Committee has been constituted to oversee the risk management process in the Company as
+required under the Companies Act, 2013 and SEBI (LODR) Regulations. The details of the Committee and its terms of
+reference are set out in the Corporate Governance Report forming part of the Board's Report. The Risk Management
+Policy h</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>17248</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>0.7688718769043267</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>['risk management']</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Amit_spinning</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>AMIT SPINNING INDUSTRIES LTD</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>5210760318.pdf</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2017-18</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>AMIT SPINNING INDUSTRIES LTD.
+CLC
+(Manufacturer onarns &amp; Govt. Recognised Trading House)
+September 27, 2018
+ESE Limited
+Stock Code. 521076
+Corporate Realationship Deptt.
+1“ Floor, New Trading Ring, Rotunda Bldg.
+PJ Towers, Dalal Street
+National Stock Exchange of India Ltd.
+Stock Code: ASIL
+Exchange Plaza
+Bandra Kurla Complex
+Bandar (E), Mumbai-400051
+Dear Sir/Madam,
+Sub:
+Submission of Annual Report for the financial year 2017-2018
+Ref:
+Regulation 34 (1) of SEBI (Listing Obligations and Disclosure Requirements) Regulations,
+Pursuant
+to
+Regulation
+(1)
+of
+SEBI
+(Listing Obligations
+and
+Disclosure Requirements)
+Regulations,
+2015,
+please find
+enclosed
+herewith Annual
+Report of the Company for the
+financial year 2017-18 duly approved and adopted by the members at the 26'h Annual General
+Meeting held on 27th September, 2018 as per the applicable provisions of the Companies Act,
+2013.
+Please take the above on record.
+Thanking you,
+Yours truly,
+For AMIT SPINNING INDUSTRIES LIMITED
+a? w.
+r \ I
+COMPLIANCE OFFICER
+W".
+Encl:
+as above.
+Regd. &amp; Corporate Office :A»60, Okhla Industrial Area, Phase-II, New Delhi 110 020 (INDIA)
+: +91—11-26385181,Emai1 :inIo@clcindia.com. www.5pemexinduslries.com
+Factory Address : Gate No. 47 &amp; 48, Sangawade Village, Kolhapur—Hupari Road, Taluka-Karveer, Distt. Kolhapur-4 l 6 202 (INDIA)
+Tel.
+BOARD OF DIRECTORS
+REGISTERED &amp; CORPORATE OFFICE
+S P Setia
+(Non-Executive / Independent Chairman)
+A-60, Okhla Industrial Area,
+Jitendra Chopra
+(Managing Director)
+Phase - II, New Delhi - 110020
+Deepak Choudhari
+(Joint Managing Director)
+Sharmila Devi Chopra (Non-Executive Director)
+Shivani Gupta
+(Non-Executive / Independent Woman Director)
+Vijay Bhan Singh
+(Non-Executive Director)
+REGISTRAR &amp; TRANSFER AGENTS
+M/s. RCMC Share Registry Pvt. Ltd.
+B-25/1, Okhla Industrial Area, Phase-II,
+Near Rana Motor, New Delhi - 110020
+PLANT
+Gat No. 47 &amp; 48, Sangavade Village
+Kolhapur - Hupari Road
+Taluka Karveer
+Dist. Kolhapur 416 202
+MAHARASHTRA
+AUDITORS
+Sunil Jain &amp; Co.
+Chartered Accountants
+New Delhi
+CHIEF FINANCIAL OFFICER
+Shreyans Rajendra Choudhari
+COMPANY SECRETARY
+Aniruddha Badkatte
+BANKERS / ARC
+AXIS Bank Limited
+JM Financial Asset Reconstruction Company Pvt. Ltd.
+INDEX
+Page No.
+Board’s Report Including
+Management Discussions &amp;
+Analysis Report
+Annexures to Boards’ Report
+Corporate Governance
+Auditor’s Report
+Balance Sheet
+Statement of Profit &amp; Loss
+Cash Flow Statement
+Notes
+26th AGM
+Date
+September 27, 2018 Time 11:30 A.M.
+Venue
+Bipin Chandra Pal Memorial Bhavan, A-81, Chittaranjan Park, New Delhi - 110 019
+Book Closure :
+Saturday, the 22nd September, 2018 to Thursday, the 27th September, 2018 (both days inclusive)
+Company’s shares are listed on BSE Ltd. and National Stock Exchange of India Ltd.
+BOARD'S REPORT
+Dear Members,
+Your Directors have great pleasure in presenting the 26th Annual Report together with Audited Statements of Accounts of
+the Company for the year ended March 31, 2018.
+FINANCIAL RESULTS:
+The summarized financial results for the year ended March 31, 2018 as compared to the previous year are as follows:
+( in Lakhs)
+FINANCIAL ANALYSIS AND PERFORMANCE REVIEW
+Due to the financial constraints the company's operations remain suspended during the year under review resulting in
+decrease in revenue from operations in the current financial year ended 31st March, 2018 of Nil as compared to Rs. 15.85
+Lakhs during the previous year ended 31st March, 2017. In addition to the above, the manufacturing unit situated at
+Kolhapur, Maharashtra stands closed with effect from 1st July, 2017 after completion of applicable legal formalities.
+As the company was declared as a Sick Company under Section 3(1)(o) of SICA 1985, SICA has been repealed w.e.f 1st
+December, 2016, and such companies were allowed to approach (NCLT) within 180 days. Accordingly, the Company had
+filed its petition before NCLT for resolution of its debts and approval of rehabilitation scheme and NCLT has pronounced
+the commencement of a corporate insolvency resolution process, against the Company w.e.f 1st August, 2017 and Mr.
+Praveen Bansal was appointed as Interim Resolution Professional to exercise management powers of the Company, in
+accordance with applicable regulations under Insolvency and Bankruptcy Code, 2016.
+Subsequently, NCLT has, vide its order dated 31st July, 2018 approved the resolution plan as submitted by Resolution
+Applicants for the Company pursuant to the Corporate Insolvency Resolution Process initiated as per the provisions of the
+Insolvency and Bankruptcy Code, 2016.
+MANAGEMENT DISCUSSION AND ANALYSIS REPORT
+The Indian textiles industry is one of the leading industries in India having evolved impressively from a domestic small
+scale industry to becoming a major employment and GDP contributor with a massive manufacturing base. It is also one
+of the largest and most important sectors of the Indian economy in terms of output, foreign exchange earnings thus
+contributing greatly to the exchequer. The Textile sector occupies a unique position as a self-reliant industry, with substantial
+value-addition at each stage of processing. It has vast potential for creation of employment opportunities in the agricultural,
+industrial, organized &amp; decentralized sectors and 5.8 million cotton farmers, 40 to 50 million people engaged in textile
+related activities in rural and urban areas, particularly for un-educated, women &amp; unskilled labour. Thus, the growth and all
+round development of this sector has a direct bearing on the development of the economy.
+Amit Spinning was producing only Cotton Yarn with a capacity of 30672 spindles. During the period under review, the
+operations of Amit Spinning were badly affected due to shortage of Working Capital. Due to the financial constraints the
+Company operations had been suspended since 11th August, 2015. In addition to the above, the manufacturing unit
+situated at Kolhapur, Maharashtra stand closed with effect from 1st July, 2017 in accordance with applicable legal provisions
+due to shortage of working capital and closing of unit is a major jolt to the Company.
+MANAGEMENT PERCEPTION ON OPPORTUNITIES, RISKS, CONCERN &amp; OUTLOOK
+The Indian government has come up with the Revised Restructured Technology Up gradation Fund Scheme (RRTUFS),
+10% capital subsidy to the specified technical textile machinery, allowing 100% FDI in the Indian textiles sector under the
+automatic route may increase the profits in the coming years, the future of the Indian textile industry looks promising,
+buoyed by both strong domestic consumption as well as export demand. With consumerism and disposable income on
+the rise, the retail sector has experienced a rapid growth in the past decade with the entry of several international players.
+Further, the Textile Ministry has also introduced a new textile policy to promote value additions which sets a target of
+doubling textile exports in next 10 years.
+Particulars
+2016-2017
+2017-2018
+Revenue from Operation
+15.85
+Other Income
+0.19
+0 .76
+Profit before depreciation, interest finance charges and tax (PBDIT)
+(3,306.26)
+(1,007.67)
+Less: Interest and Finance Charges
+86.17
+1.86
+Less: Depreciation
+269.68
+296.82
+Profit/(Loss) before Tax (PBT)
+(3,662.11)
+(1,306.34)
+Less : Tax Expense/Deferred Tax
+Profit/(Loss) after Tax (PAT)
+(3,662.11)
+(1,306.34)
+Other Comprehensive Income
+(16.08)
+Total Comprehensive Income
+(3,662.11)
+(1,322.42
+The major factors hindering progress of the textiles industry are Increase in the power costs, higher transaction costs,
+high cost of labour and general increase in input costs, thus the industry has to concentrate on cost reduction exercises
+and improvement in efficiency. Another key challenge presently is the Fiber/Raw Material cost, which is increasing
+abruptly and increase is not fully absorbed in the yarn prices and accordingly yarn spinners are hit the most in the entire
+textile chain. Due to fluctuating prices and uncertainties in the foreign exchange market, increase in power cost, introduction
+of GST and lack of adequate working capital, the EBITA levels may remain stagnant during the year.
+Further, to overcome the losses promptly in this challenging scenario, the Management is keeping a close watch on
+various threats/risks facing the company and taking all appropriate steps to restart of manufacturing unit.
+With much awaited / impending approval of Resolution Plan of the Company by NCLT and with the continued support and
+co-operation of company's bankers, management believes that your Company would again resume production, optimally
+utilize capacities, and generate increasing sales volumes, margins in due course and the management is confident of a
+turnaround of the company in near future.
+SEGMENT-WISE PERFORMANCE
+Amit Spinning Industries Ltd. (ASIL) being a cotton yarn manufacturer has only one business segment. On the basis of
+geographical categorization of market, ASIL identified two segments i.e. exports and domestic.
+During the year under review, Company has not manufactured yarn.
+SUBSIDIARY COMPANIES, JOINT VENTURES AND ASSOCIATE COMPANIES
+As there are no subsidiaries/ associates / joint ventures of the Company, the provisions contained in Companies Act,
+2013/SEBI (LODR) Regulations relating to subsidiaries are not applicable.
+DIVIDEND
+During the year under review, the Company has no distributable profits hence directors regret their inability to recommend
+any dividend for financial period 2017-18.
+TRANSFER TO RESERVES
+During the year, the Company has not transferred any amount to reserves.
+SHARE CAPITAL
+The Company's Authorized Share Capital as on 31st March, 2018 stands at Rs. 25,00,00,000/- and issued &amp; paid up
+capital as on 31st March, 2018 stands at Rs. 20,58,48,335/- divided into 4,11,69,667 fully paid up equity shares of Rs. 5/
+- each. During the year, under review, the Company has not issued any share(s). Further the Company has not issued any
+share with differential Voting Rights/Sweat Equity shares/under Stock Option Scheme (ESOS) earlier and during the year.
+The Company has no scheme of provision of money for purchase of its own shares by employees or by trustees for the
+benefit of employees. Hence the details under rule 16 (4) of Companies (Share Capital and Debentures) Rules, 2014 are
+not required to be disclosed.
+DIRECTORS AND KEY MANAGERIAL PERSONNEL
+(a) Change in Directors and Key Managerial Personnel
+Mr. Jitendra kumar Goutamchand Chopra has been appointed as an Additional Director and designated as Executive
+Managing Director on the Board of the Company with effect from 10th August, 2018.
+Mr. Deepak Chaganlal Choudhari has been appointed as an Additional Director and designated as Executive Joint Managing
+Director on the Board of the Company with effect from 10th August, 2018.
+Mrs. Sharmila Devi J Chopra has been appointed as a Woman Non-Executive Director on the Board of the Company with
+effect from 10th August, 2018.
+Mr. Aniruddha Badkatte has been appointed as a Company Secretary of the Company with effect from 10th August, 2018.
+Mr. Shreyans Rajendra Choudhari has been appointed as a Chief Financial Officer of the Company with effect from 10th
+August, 2018.
+Ms. Shifali has been appointed as compliance officer of the Company w.e.f 13th April, 2018 in place of Mr. Bharat Kapoor,
+who has resigned w.e.f 10th April, 2018.
+Brief resume of the Directors proposed to be appointed/re-appointed, nature of their expertise in specific functional areas
+and names of the companies in which they hold directorship and membership/chairmanships of the Board or its Committees,
+as stipulated under SEBI (LODR) Regulations entered into by the Company with stock exchanges in India, is provided in
+the notice of 26th Annual General Meeting.
+(b) Number of Meetings of the Board
+Four meetings of the Board were held during the year. The detailed information regarding meetings of the Board held
+during the year is mentioned in the Corporate Governance Report which forms part to this report.
+(c) Declaration by Independent Directors
+All Independent Directors have given declarations that they meet the criteria of independence as laid down under Section
+149(6) of the Companies Act, 2013 and SEBI (LODR) Regulations.
+(d) Annual Evaluation by the Board
+Pursuant to the provisions of the Companies Act, 2013 and SEBI (LODR) Regulations, the Board has carried out an
+annual performance evaluation of its own performance, the directors individually as well as its Committees. The manner
+in which the evaluation has been carried out has been explained in the Corporate Governance Report.
+(e) Remuneration Policy
+The Board has, on the recommendation of the Nomination &amp; Remuneration Committee framed a policy for selection and
+appointment of Directors, Senior Management and their remuneration. The Remuneration Policy is enumerated in the
+Corporate Governance Report. During the year, neither the Managing Director nor the Whole-time Directors of the Company
+received any remuneration or commission from any of its subsidiaries.
+DIRECTORS' RESPONSIBILITY STATEMENT
+Pursuant to the requirement of Section 134(3) (c) of the Companies Act, 2013, with respect to Directors' Responsibility
+Statement, it is hereby confirmed that:
+(a) in the preparation of the annual accounts for the financial year ended 31st March, 2018, the applicable accounting
+standards had been followed along with proper explanation relating to material departures;
+(b) the directors had selected such accounting policies and applied them consistently and made judgments and estimates
+that are reasonable and prudent so as to give a true and fair view of the state of affairs of the company as at March 31,
+2018 and of the profit and loss of the company for that period;
+(c) the directors had taken proper and sufficient care for the maintenance of adequate accounting records in accordance
+with the provisions of the Companies Act, 2013 for safeguarding the assets of the company and for preventing and
+detecting fraud and other irregularities;
+(d) the directors had prepared the annual accounts on a going concern basis; and
+(e) the directors had laid down internal financial controls to be followed by the company and that such internal financial
+controls are adequate and were operating effectively.
+(f)
+the directors had devised proper systems to ensure compliance with the provisions of all applicable laws and that
+such systems were adequate and operating effectively.
+RELATED PARTY TRANSACTIONS
+None of the transactions with related parties falls under the scope of section 188(1) of the Act. All related party transactions
+that were entered into during the financial year were on an arm's length basis and were in the ordinary course of business.
+There were no materially significant related parties transactions entered into by the Company with Holding Company/
+Promoters, Directors, Key Managerial Personnel or other designated persons which may have a potential conflict with the
+interest of the Company at large.
+Prior omnibus approval of the Audit Committee was obtained for Related Party Transactions for the year ended 31st
+March, 2018 and for transactions proposed to be entered into with related parties for the financial year 2018-19 were
+placed before the said committee and consent of the said committee was obtained.
+The policy on Related Party Transactions as approved by the Board has been uploaded on the website www.spentex.net.
+None of the Directors has any pecuniary relationships or transactions vis-a-vis the Company. Since all related party
+transactions entered into by the Company were in ordinary course of business and were on an arm's length basis, form
+AOC - 2 is not applicable to the Company.
+MATERIAL CHANGES AND COMMITMENTS AFFECTING THE FINANCIAL POSITION BETWEEN THE DATE OF THE
+BOARD REPORT AND END OF FINANCIAL YEAR
+During the year under review, the company's operations remain suspended due to the financial constraints and in addition
+to the above, the manufacturing unit situated at Kolhapur, Maharashtra stands closed with effect from 1st July, 2017 after
+completion of applicable legal formalities.
+NCLT has, vide its order dated 31st July, 2018 approved the resolution plan as submitted by Resolution Applicants for the
+Company pursuant to the Corporate Insolvency Resolution Process in respect of the Company under Insolvency and
+Bankruptcy Code, 2016.
+SIGNIFICANT AND MATERIAL ORDERS PASSED BY THE REGULATORS OR COURTS.
+NCLT has, vide its order dated 31st July, 2018 approved the resolution plan as submitted by Resolution Applicants for the
+Company pursuant to the Corporate Insolvency Resolution Process in respect of the Company under Insolvency and
+Bankruptcy Code, 2016.
+AUDITORS AND AUDITORS REPORT
+(a) Statutory Auditors
+Pursuant to the provisions of Section 139 of the Companies Act, 2013 read with the rules framed thereunder, M/s Sunil
+Jain &amp; Co., Chartered Accountants, (Firm Registration No. 002855N) was appointed as Statutory Auditor of the Company
+at the 22nd Annual General Meeting held on 11.09.2014, to hold office till the conclusion of the 26th Annual General
+Meeting to be held in the Calendar Year 2018, subject to ratification of their appointment at every annual general meeting.
+The terms of M/s Sunil Jain &amp; Co., Chartered Accountants, will expire at the ensuing Annual General Meeting.
+The Audit Committee and Board of Directors, at their meeting held on 10th August, 2018, have recommended the
+appointment of M/s Sanjay Vhanbatte &amp; Company, Chartered Accountants, (Firm Registration No. 112996W) as statutory
+auditors of the Company in place of retiring Auditor, to hold office from the conclusion of 26th Annual General Meeting till
+the conclusion of 31st Annual General Meeting. The Company has received a confirmation from M/s Sanjay Vhanbatte &amp;
+Company, Chartered Accountants to the effect that their appointment, if made, at the ensuing AGM would be in terms of
+Sections 139 and 141 of the Companies Act, 2013 and rules made there under and that they are not disqualified for the
+appointment. Their appointment is being placed for consideration of members in ensuing Annual General Meeting.
+Auditor's Report
+Statutory Auditors i.e, M/s Sunil Jain &amp; Co., have submitted Auditors' Report on the accounts of the Company for the
+period ended 31st March 2018. The Auditor's Report read with Notes to Accounts is self-explanatory and does not call for
+any further explanation under Section 134 of the Companies Act, 2013. Directors' response to the various observations of
+the auditors made in their report, have been explained wherever necessary through appropriate notes to accounts
+(b) Cost Auditor:
+The Company having been declared as a sick company under repealed SICA and having not produced any yarn in the
+year 2017-18, the Companies (Cost Records and Audit Rules), 2014 is not applicable to the Company.
+(c) Secretarial Auditor &amp; Audit Report:
+Pursuant to provisions of Section 204 of the Companies Act, 2013, the Company has appointed M/s. Loveneet Handa &amp;
+Associate, Practicing Company Secretary (having CP No. 10753 &amp; Membership No. 9055) as Secretarial Auditor to carry
+out the secretarial audit for the financial year 2017-18.
+The Secretarial Audit Report for the financial year ended March 31, 2018 is annexed herewith marked as Annexure 1 to
+this Report.
+The qualifications/observations/remarks made by the Secretarial Auditors and management's view thereon are given in
+their Report attached hereto.
+INTERNAL CONTROL SYSTEMS AND ADEQUACY
+The Company has established adequate internal control systems, commensurate with its size and nature of business and
+such systems are periodically audited, verified and reviewed for their validity, considering the changing business scenario
+from time to time, the Audit Committee of the Board of Directors reviews the adequacy and effectiveness of internal
+control systems and suggests improvement for strengthening them.
+EXTRACT OF THE ANNUAL RETURN
+The details forming part of the extract of annual return in Form MGT-9 as required under Section 92(3) of the Companies
+Act and Rule 12 of the Companies (Management and Administration) Rules, 2014 is available on the website
+www.spentex.net
+CONSERVATION OF ENERGY, TECHNOLOGY ABSORPTION AND FOREIGN EXCHANGE EARNINGS AND OUTGO.
+As there is no operation/production during the year under review, the information as required to be disclosed under
+Section 134(3)(m) of the Companies Act, 2013 read with Rule, 8 of the Companies (Accounts) Rules, 2014 is not applicable.
+PARTICULARS OF EMPLOYEES
+The statement containing particulars of employees as required under section 197(12) of the Act read with Rule 5(2) &amp; 5(3)
+of the companies (Appointment and Remuneration of Managerial Personnel) Rules, 2014 as amended, shall be made
+available to any shareholder on a specific request made by him in writing on or before 27th September, 2018
+DEPOSITS
+The Company has not accepted or renewed any deposit during the year and there are no outstanding and/or overdue
+deposits as at 31st March, 2018.
+PARTICULARS OF LOANS, GUARANTEES OR INVESTMENTS
+Details of loans, Guarantees and Investments covered under the provision of Section 186 of the Companies Act, 2013 are
+given in the notes to the Financial Statements.
+RISK MANAGEMENT
+A Risk Management Committee has been constituted to oversee the risk management process in the Company as
+required under the Companies Act, 2013 and SEBI (LODR) Regulations. The details of the Committee and its terms of
+reference are set out in the Corporate Governance Report forming part of the Board's Report. The Risk Management
+Policy has also been hosted on the website of the company
 VIGIL MECHANISM
-The Company has framed and implemented a vigil mechanism named as Whistle Blower Policy to deal with instances of fraud and
-mismanagement, if any. The details of the Whistle Blower Policy are provided in the Corporate Governance Report and also hosted on
-the website of the Company.
-During the year under review, there were no cases filed pursuant to the Sexual Harassment of Women at Workplace (Prevention,
-Prohibition and Redressal) Act, 2013.
+The Company has framed and implemented a vigil mechanism named as Whistle Blower Policy to deal with instances of
+fraud and mismanagement, if any. The details of the Whistle Blower Policy are provided in the Corporate Governance
+Report and also hosted on the website of the Company.
+During the year under review, the Company has an Internal Complaint Committee as required under Sexual Harassment
+of Women at Workplace (Prevention, Prohibition and Redressal) Act, 2013 and, there were no compliant received during
+the year.
 HUMAN RESOURCES/INDUSTRIAL RELATIONS
-A Fundamental concept embodied in the company's code of conduct is to provide working environment that motivate employees to be
-productive and innovative and provide opportunities for employee training and development to maximize personal potential and
-develop careers within the Group. The Company values the involvement of its employees and keep them informed on matters affecting
-them as employees and factors relevant to the company's performance and other employee related issues on a non discriminatory
-basis.
-The Board of Directors place on record the active, dedicated and valuable contribution made by employees of the Company at all levels
-with regard to the affairs of the Company. The Industrial relations remained cordial within the Company.
+A fundamental concept embodied in the company's code of conduct is to provide working environment that motivate
+employees to be productive and innovative and provide opportunities for employee training and development to maximize
+personal potential and develop careers within the Company. The Company values the involvement of its employees and
+keep them informed on matters affecting them as employees and factors relevant to the company's performance and
+other employee related issues on a non discriminatory basis.
+The Board of Directors place on record the active, dedicated and valuable contribution made by employees of the Company
+at all levels with regard to the affairs of the Company. The Industrial relations remained cordial within the Company.
 FRAUD REPORTING
-During the year no fraud has been reported to the Audit Committee / Board.
+During the year Statutory Auditors has not found any instance of fraud committed against the Company by its employees
+or officers and accordingly, reporting to the Audit Committee or Central Government is not required.
 INFORMATION TECHNOLOGY
-Information Technology continues to be an integral part of your company's business strategy. The Company is working on SAP
-platform integrating its business processes, financial parameters, customer transactions and people, effectively on real time basis.
+Information Technology continues to be an integral part of your company's business strategy. The Company is working on
+SAP platform integrating its business processes, financial parameters, customer transactions and people, effectively on
+real time basis.
 CHANGE IN THE NATURE OF BUSINESS
 There is no change in the nature of the business of the company.
 CORPORATE GOVERNANCE AND MANAGEMENT DISCUSSION AND ANALYSIS
-As stipulated under SEBI (LODR) Regulations, 2015, a report on Corporate Governance is attached separately as a part of the Annual
-Report and the Management Discussion and Analysis (MD &amp; A) is included in this report so that duplication and overlap between
-Boards' Report and a separate MD &amp; A is avoided and the entire information is provided in a composite and comprehensive manner.
+As stipulated under SEBI (LODR) Regulations entered into with Stock Exchanges, a report on Corporate Governance is
+attached separately as a part of the Annual Report and the Management Discussion and Analysis (MD &amp; A) is included in
+this report so that duplication and overlap between Directors' Report and a separate MD &amp; A is avoided and the entire
+information is provided in a composite and comprehensive manner.
 LISTING OF SHARES
-Presently Company's shares are listed and traded at the BSE Limited, Mumbai (BSE) and National Stock Exchange of India, Mumbai
-(NSE). Due to closure of operations of manufacturing unit and non approval of Rehabilitation Scheme by concerned authority the
-company has not paid the Annual Listing Fee for the financial year 2015-16 and 2016-17 to BSE &amp; NSE and Company would be in a
-position to pay the same only after infusion of funds pursuant and subsequent to the approval of Rehabilitation Scheme.
+Presently Company's shares are listed and traded at the BSE Limited, Mumbai (BSE) and National Stock Exchange of
+India, Mumbai (NSE). Due to closure of the manufacturing unit situated at Kolhapur the company could not pay the Annual
+Listing Fee to BSE &amp; NSE.
 CONCLUSION
-Your company is presently going through challenging and difficult period due to market and financial constraints. It has already been
-declared as a Sick Company under Sick Industrial Companies (Special Provisions) Act, 1985 by BIFR vide its order dated 18th
-July'2012, and UCO Bank has been appointed as an Operating Agency to work out DRS for the Company in consultation with lenders.
-It is however expected, on Company receiving BIFR approval for its DRS, it would be in a better position to augment its production and
-sales, by utilizing its capacities optimally. UCO Bank has assigned its debt to JM Financial Asset Reconstruction Company Pvt. Ltd.
-Acknowledgments
-Your Directors place on record their sincere thanks to bankers, financial institutions business associates, consultants, customers,
-suppliers, contractors and various Government Authorities for their continued support extended to your Company's activities during
-the year under review. Your Directors also gratefully acknowledge the continuing support of the shareholders and the confidence
-reposed by them in the company
-Place New Delhi
-Date : August 9, 2016
-On behalf of the BOARD OF DIRECTORS
+Your company was going through challenging and difficult period due to market and financial constraints. The Resolution
+Applicants have submitted the Resolution Plans for the revival of the Company, out of which one Resolution Plan has
+been approved by the Committee of Creditors at their meeting held on 26th April, 2018 and the same was subsequently
+approved by the NCLT, vide its order dated 31st July, 2018. It is however expected, that with approval of Resolution Plan
+by NCLT, It would be in a better position to augment its production and sales by utilizing its capacities optimally.
+Acknowledgements
+Your Directors place on record their sincere thanks to bankers, financial institutions business associates, consultants,
+customers, suppliers, contractors and various Government Authorities for their continued support extended to your
+Companies activities during the year under review. Your Directors also acknowledge gratefully the shareholders for their
+support and confidence reposed on the Company.
+For &amp; on behalf of the Board
 Sd/-
-S P SETIA
-CHAIRMAN
-Annexure - 1 to the Director's Report
-Form for Disclosure of particulars of contracts/arrangements entered into by the company with related parties referred to in sub section
-(1) of section 188 of the Companies Act, 2013 including certain arms length transaction under third proviso thereto.
-1. Details of contracts or arrangements or transactions not at Arm's length basis – N.A.
-2. Details of material contracts or arrangements or transactions at Arm's length basis.
-FORM NO. AOC -2
-(Pursuant to clause (h) of sub-section (3) of section 134 of the Act and
-Rule 8(2) of the Companies (Accounts) Rules, 2014)
-SL. No.
-Particulars
-Details
-Name (s) of the related party &amp; nature of relationship
-Spentex Industries Ltd. (Holding Company)
-Nature of contracts/arrangements/transaction
-Sale/Purchase of godds/services
-Duration of the contracts/arrangements/transaction
-Salient terms of the contracts or arrangements or
-Ongoing transactions on normal business terms.
-transaction including the value, if any
-Value of all transactions is Rs. 50,71,101/-
-Date of approval by the Board
-25.05.2016
-Amount paid as advances, if any
-Annexure-2 to the Director's Report
+S.P. Setia
+Chairman
+Place : New Delhi
+Date : 10th August, 2018
+Annexure - 1 to the Director’s Report
 Form No. MR-3
 SECRETARIAL AUDIT REPORT
-FOR THE FINANCIAL YEAR ENDED ON 31ST MARCH, 2016
-(Pursuant to section 204(1) of the Companies Act, 2013 and Rule No. 9
-of the Companies (Appointment and Remuneration of Managerial Personnel) Rules, 2014)
+FOR THE FINANCIAL YEAR ENDED ON 31ST MARCH, 2018
+(Pursuant to section 204(1) of the Companies Act, 2013 and Rule No. 9 of the Companies (Appointment and
+Remuneration of Managerial Personnel) Rules, 2014)
 To,
 The Members,
 Amit Spinning Industries Limited
-We have conducted the Secretarial Audit of the compliance of applicable statutory provisions and the adherence to good corporate
-practices by M/s Amit Spinning Industries Limited (hereinafter called the Company). Secretarial Audit was conducted in a manner
-that provided us a reasonable basis for evaluating the corporate conducts/statutory compliances and expressing our opinion thereon.
-Based on our verification of the Company's books, papers, minute books, forms and returns filed and other records maintained by the
-Company and also information provided by the Company, its officers, agents and authorized representatives during the conduct of
-secretarial audit, We hereby report that in our opinion, the company has, during the audit period covering the financial year ended on
-31st March, 2016, complied with the statutory provisions listed hereunder and also that the Company has proper Board-processes and
-compliance-mechanism in place to the extent, in the manner and subject to the reporting made hereinafter:
-We have examined the books, papers, minute books, forms and returns filed and other records maintained by M/s. Amit Spinning
-Industries Limited as given in Annexure I for the financial year ended on 31st March, 2016 according to the provisions of:
+We have conducted the Secretarial Audit of the compliance of applicable statutory provisions and the adherence to good
+corporate practices by M/s Amit Spinning Industries Limited (hereinafter called the Company). Secretarial Audit was
+conducted in a manner that provided us a reasonable basis for evaluating the corporate conducts/statutory compliances
+and expressing our opinion thereon.
+Based on our verification of the Company's books, papers, minute books, forms and returns filed and other records
+maintained by the Company and also information provided by the Company, its officers, agents and authorized
+representatives during the conduct of secretarial audit, we hereby report that in our opinion, the company has, during the
+audit period covering the financial year ended on 31st March, 2018, complied with the statutory provisions listed hereunder
+and also that the Company has proper Board-processes and compliance-mechanism in place to the extent, in the manner
+and subject to the reporting made hereinafter:
+We have examined the books, papers, minute books, forms and returns filed and other records maintained by M/s Amit
+Spinning Industries Limited as given in Annexure I for the financial year ended on 31st March, 2018 according to the
+provisions of:
+I.
+The Companies Act, 2013 (the Act) and the rules made there under;
+II.
+The Securities Contracts (Regulation) Act, 1956 ('SCRA) and the rules made there under;
+III. The Depositories Act, 1996 and the Regulations and Bye-laws framed there under;
+IV. Foreign Exchange Management Act, 1999 and the rules and regulations made there under to the extent of Foreign
+Direct Investment, Overseas Direct Investment and External Commercial Borrowings;
+V.
+The Regulations and Guidelines prescribed under the Securities and Exchange Board of India Act, 1992 ('SEBI Act') viz.:
+VI. The Securities and Exchange Board of India (Substantial Acquisition of Shares and Takeovers) Regulations, 2011;
+VII. The Securities and Exchange Board of India (Prohibition of Insider Trading) Regulations, 2015;
+VIII.The Securities and Exchange Board of India (Issue of Capital and Disclosure Requirements) Regulations, 2009;
+IX. The Securities and Exchange Board of India (Share Based Employee Benefits) Regulations, 2014); (N.A.)
+X.
+The Securities and Exchange Board of India (Issue and Listing of Debt Securities) Regulations. 2008; (N.A.)
+XI. The Securities and Exchange Board of India (Registrars to an Issue and Share Transfer Agents) Regulations, 1993
+regarding the Companies Act and dealing with client;
+XII. The Securities and Exchange Board of India (Delisting of Equity Shares) Regulations, 2009; (N.A.) and
+XIII.The Securities and Exchange Board of India (Buyback of Securities) Regulations, 1998. (N.A.)
 (i)
-The Companies Act, 2013 (the Act) and the rules made there under;
-(ii)
-The Securities Contracts (Regulation) Act, 1956 ('SCRA) and the rules made there under;
-(iii) The Depositories Act, 1996 and the Regulations and Bye-laws framed there under;
-(iv) Foreign Exchange Management Act, 1999 and the rules and regulations made there under to the extent of Foreign Direct
-Investment, Overseas Direct Investment and External Commercial Borrowings;
-(v) The Regulations and Guidelines prescribed under the Securities and Exchange Board of India Act, 1992 ('SEBI Act') viz.:
-(a) The Securities and Exchange Board of India (Substantial Acquisition of Shares and Takeovers) Regulations, 2011;
-(b) The Securities and Exchange Board of India (Prohibition of Insider Trading) Regulations, 2015;
-(c) The Securities and Exchange Board of India (Issue of Capital and Disclosure Requirements) Regulations, 2009;
-(d) The Securities and Exchange Board of India (Employee Stock Option Scheme and Employee Stock Purchase Scheme)
-Guidelines, 1999; (N.A.)
-(e) The Securities and Exchange Board of India (Issue and Listing of Debt Securities) Regulations. 2008; (N.A.)
-(f)
-The Securities and Exchange Board of India (Registrars to an Issue and Share Transfer Agents) Regulations, 1993 regarding
-the Companies Act and dealing with client;
-(g) The Securities and Exchange Board of India (Delisting of Equity Shares) Regulations, 2009; (N.A.) and
-(h) The Securities and Exchange Board of India (Buyback of Securities) Regulations, 1998. (N.A.)
-(vi) OTHER APPLICABLE ACTS
+OTHER APPLICABLE ACTS
 (a) Factories Act, 1948
 (b) Payment Of Wages Act, 1936, and rules made there under,
 (c) The Minimum Wages Act, 1948, and rules made there under,
@@ -4920,508 +6209,110 @@
 (i)
 Food Safety and Standards Act, 2006, and rules made there under.
 (j)
-Environment (Protection) Act, 1986
+Environment (Protection) Act, 1986.
 We have also examined compliance with the applicable clauses of the following:
 1.
 Secretarial Standards issued by The Institute of Company Secretaries of India.
 2.
-The Listing Agreements entered into by the Company with Bombay Stock Exchange and National Stock Exchange.
+The Listing Agreements entered into by the Company with BSE Limited and National Stock Exchange of India Limited.
 3.
 Securities and Exchange Board of India (Listing Obligations and Disclosure Requirements) Regulations, 2015
-During the period under review the Company has complied with the provisions of the Act, Rules, Regulations, Guidelines, Standards,
-etc. mentioned above.
+(hereinafter called "SEBI Listing Regulations").
+During the year under review, the Company has complied with the provisions of the Act, Rules, Regulations, Guidelines,
+Standards, etc. mentioned above.
 We further report that:
 1.
-The Board of Directors of the Company was not constituted with proper balance of Executive Directors, Non-Executive/
-Independent Directors as on March 31, 2016. However, as on June 30, 2016, the composition of the Board of Directors of the
-Company is in conformity with the requirements as stipulated under SEBI (LODR) Regulations, 2015 and the Companies Act,
-2013 and rules framed there under.
+The Board of Directors of the Company is not constituted with proper balance of Executive Directors and Non-
+Executive Directors. There is no Executive Director on the Board of the Company. The composition of Independent
+Directors on the Board of Directors of the Company is in conformity with the requirements as stipulated under SEBI
+Listing Regulations and the Companies Act, 2013 and rules framed there under.
 2.
-Adequate notice is given to all directors to schedule the Board Meetings, agenda and detailed notes on agenda were sent at least
-seven days in advance and a system exists for seeking and obtaining further information and clarifications on the agenda items
-before the meeting and for meaningful participation at the meeting.
+The Company is required to appoint a Whole Time Company Secretary as per the provisions of Section 203 of the
+Companies Act, 2013 read with Companies (Appointment and Remuneration of Managerial Personnel) Rules, 2014
+and SEBI Listing Regulations, however, there is no Whole Time Company Secretary of the Company, during the
+financial year ended on 31st March, 2018.
 3.
-Majority decision is carried through while the dissenting members' views are captured and recorded as part of the minutes.
+Mr. Malpeddi Nagnath S, the Chief Financial Officer (CFO) of the Company has resigned w.e.f. 01st August, 2017 and
+no person has further been appointed as CFO of the Company under Section 203 of the Companies Act, 2013.
 4.
-There are adequate systems and processes in the company commensurate with the size and operations of the company to
-monitor and ensure compliance with applicable laws, rules, regulations and guidelines.
+As per provisions of Companies Act, 2013 and Company rules 2014 read with various Regulations of SEBI Listing
+Regulations, 2015, the Company has constituted the Risk Management Committee, Stakeholders Relationship Committee,
+Audit Committee, Nomination &amp; Remuneration Committee and uploaded applicable policies at Company's website.
 5.
-The Company has well maintained all the Statutory Registers i.e. Register of Members, Register of Charges, Register of Directors
-Shareholding etc. mandatory to be maintained under Companies Act, 2013.
+The number of members of Audit Committee and Nomination and Remuneration Committee of the Company was less
+than three from 01st August, 2017 to 31st December, 2017 due to the resignation of Mr. K. Sankaramani, Independent
+Director of the Company, which was not in accordance with SEBI Listing Regulations and Section 177 and 178 of the
+Companies Act, 2013.
 6.
-The Company was unable to pay off listing fees to stock exchanges; NSE &amp; BSE, for the financial year 2015-16 &amp; 2016-17. The
-Rehabilitation Scheme filed by the company with BIFR is yet to be considered and approved. The management has no option but
-continue to keep the manufacturing unit situated at Kolhapur, Maharashtra, inoperative, as before for the time being, due to
-financial constraints and non-availability of working capital.
+The company was unable to pay off the Listing Fees of National Stock Exchange (NSE) and Bombay Stock Exchange
+(BSE) for the Financial Year 2016-2017 and 2017-18 due to financial constraints. The Company has received Letters,
+Reminders, E mails from the NSE &amp; BSE for the payment of unpaid listing fees.
 7.
-The Company has paid all the statutory dues except dues related to EPF (Employee Provident Fund) and Service Tax for the
-financial year 2015-2016 due to financial constraints.
+In view of adoption of IND-AS by the Company for the first time w.e.f 1st April, 2017, the Company has submitted the
+Financial Results for the quarter ended 30th June, 2017 on 23rd September, 2017 as against the due date of 14th
+September, 2017, hence the BSE Ltd. and National Stock Exchange Ltd. has imposed SOP (Standard Operating
+Procedure) fine for the non compliance of Regulation 33 of SEBI Listing Regulations. The Company has received
+letters, reminders from the stock exchanges for the payment of same with the statement that if the same would not be
+paid within stipulated time, then, the holding of the promoter and promoter group in other securities shall be freezed,
+in consequence.
 8.
-The Company has complied with all the provisions of SEBI (Listing obligations and Disclosure Requirements) regulation, 2015
-and SEBI (Insider Trading) Regulations, 2015 in respect to opening trading window, Company intimated 24 hours instead of 48
-hours.
-9.
-On July 18, 2012 Board for Industrial &amp; Financial Reconstruction declared the company as Sick Industrial Company under Section
-3(1)(o) of SICA, 1985 &amp; has also appointed Operating Agency to prepare a rehabilitation scheme.
-10. As per provisions of Companies Act, 2013 and Company rules 2014 read with various clauses of Listing Agreement/SEBI (Listing
-Obligation and Disclosure Requirements) Regulations, 2015, the Company has constituted the Risk Management Committee,
-Stakeholders Relationship Committee, Audit Committee, Nomination &amp; Remuneration Committee and uploaded applicable
-policies at Company's website.
-11. The Company has appointed Mr. Malpeddi Nagnath S as Chief Financial Officer of the Company in the Board Meeting held on 08-
-02-2016 and filed all necessary documents with Registrar of Companies except MR-1 till today. At the time of appointment of CFO,
-Form MR-1 is applicable, however, the same have now been dispensed by Ministry of Corporate Affairs.
-During the period under review the Company has complied with the provisions of the Act, Rules, Regulations, Guidelines, Standards,
-etc. mentioned above and there were no specific events / actions having a major bearing on the company's affairs
-For Loveneet Handa &amp; Associates
-(Practicing Company Secretary)
-Sd/-
-Place: New Delhi
-Loveneet Handa
-Dated: August 03, 2016
-Annexure - I
-Documents examined/verified while conducting secretarial audit:
-(a) Books ,Papers, as per Section 2 (12) of Companies Act, 2013,“book and paper” and “book or paper” include books of account,
-deeds, vouchers, writings, documents, minutes and registers maintained on paper or in electronic form. (Registers Maintained by
-RTA)
-(b) Memorandum of association
-(c) Articles of association
-(d) Certificate of Incorporation
-(e) Audited balance sheet(s)
-(f)
-Statutory Registers maintained by the Company i.e. Register of Members/ Register of Charges/ Register of Directors
-Shareholding/ Register of Contract/ Register of Investment, Register of Director Shareholdings, Register of Contracts of the Co.
-and firms in which directors etc are interested, Common Seal Register etc.
-(g) Minutes of the Board meetings, Annual General Meeting, Stakeholders Relationship Committee Meeting, and Audit Committee
-Meeting, Nomination &amp; Remuneration Committee Meeting.
-(h) Notice of calling Annual General Meeting along with the explanatory statement.
-(i)
-Copy of documents related to the appointment/Resignation of Statutory Auditor of the company
-(J) Copy of Internal Audit Report given by Internal Auditor appointed u/s 138 of Companies Act, 2013.
-I.
-REGISTRATION AND OTHER DETAILS:
-FORM NO. MGT 9
-EXTRACT OF ANNUAL RETURN
-as on financial year ended on 31.03.2016
-Pursuant to Section 92 (3) of the Companies Act, 2013 and rule 12(1) of the Company
-(Management &amp; Administration ) Rules, 2014.
-Annexure - 3 to the Director's Report
-i)
-CIN
-ii)
-Registration Date
-18.11.1991
-iii) Name of the Company
-Amit Spinning Industries Limited
-iv) Category/Sub-category of the Company
-Public Limited Company
-v)
-Address of the Registered office &amp; contact details
-A - 60, Okhla Industrial Area, Phase - II, New Delhi - 110020;
-vi) Whether listed company
-Yes
-vii) Name, Address &amp; contact details of
-RCMC Share Registry Pvt. Ltd., B-25/1, Okhla Industrial Area,
-the Registrar &amp; Transfer Agent, if any
-II.
-PRINCIPAL BUSINESS ACTIVITIES OF THE COMPANY
-All the business activities contributing 10 % or more of the total turnover of the company shall be stated:-
-Sr. No.
-Name &amp; Description of main products/services
-NIC Code of the
-% to total turnover
-Product /service
-of the company
-Yarn
-III.
-PARTICULARS OF HOLDING , SUBSIDIARY &amp; ASSOCIATE COMPANIES
-Sr.
-NAME AND ADDRESS OF
-CIN/GLN
-HOLDING/
-% OF
-APPLICABLE
-No.
-THE COMPANY
-SUBSIDIARY/
-SHARES
-SECTION
-ASSOCIATE
-HELD
-Spentex Industries Limited
-Holding
-50.96%
-2 (46)
-A - 60, Okhla Industrial Area,
-Phase - II, New Delhi - 110020
-A. Promoters
-(1)Indian
-a) Individual/HUF
-0.00
-0.00
-0.00
-b) Central Govt. or
-0.00
-0.00
-0.00
-State Govt.
-c) Bodies Corporates
-20,981,077
-20,981,077
-50.96
-20,981,077
-20,981,077
-50.96
-0.00
-d) Bank/FI
-0.00
-0.00
-0.00
-e) Any other
-0.00
-0.00
-0.00
-SUB TOTAL:(A) (1)
-50.96
-20,981,077
-20,981,077
-50.96
-0.00
-IV. SHAREHOLDING PATTERN (Equity Share capital Break up as % to total Equity)
-i)
-Category wise shareholding
-Category of
-No. of Shares held at the beginning
-No. of Shares held at the end
-%change
-Shareholders
-of the year
-of the year
-during
-Demat
-Physical
-Total
-% of
-Demat
-Physical
-Total
-% of
-the year
-Total
-Total
-Shares
-Share
-(2)Foreign
-a) NRI- Individuals
-0.00
-0.00
-0.00
-b) Other Individuals
-0.00
-0.00
-0.00
-c) Bodies Corporates
-0.00
-0.00
-0.00
-d) Banks/FI
-0.00
-0.00
-0.00
-e) Any other
-0.00
-0.00
-0.00
-SUB TOTAL (A) (2)
-0.00
-0.00
-0.00
-Total Shareholding of
-20,981,077
-20,981,077
-50.96
-20,981,077
-20,981,077
-50.96
-0.00
-Promoter (A) = (A)(1)+
-(A)(2)
-B. PUBLIC
-SHAREHOLDING
-(1)Institutions
-a) Mutual Funds
-0.00
-0.00
-0.00
-b) Banks/FI
-0.00
-0.00
-0.00
-C) Central Govt
-0.00
-0.00
-0.00
-d) State Govt.
-0.00
-0.00
-0.00
-e) Venture Capital Fund
-0.00
-0.00
-0.00
-f) Insurance Companies
-2,000
-2,000
-0.00
-2,000
-2,000
-0.00
-0.00
-g) FIIS
-0.00
-0.00
-0.00
-h) Foreign Venture
-0.00
-0.00
-0.00
-Capital Funds
-i) Others (specify)
-0.00
-0.00
-0.00
-Foreign Bank
-SUB TOTAL (B)(1):
-2,000
-2,100
-0.01
-2,000
-2,100
-0.01
-0.00
-(2)Non Institutions
-a) Bodies Corporates
-i) Indian
-860,293
-7,900
-868,193
-2.11
-799,811
-7,900
-807,711
-1.96
--0.15
-ii) Overseas
-0.00
-0.00
-0.00
-b) Individuals
-i) Individual shareholders
-4,343,826
-1,748,240
-6,092,066
-14.80
-6,718,997
-16.32
-1.52
-holding nominal share
-capital upto Rs.1 lakhs
-ii) Individuals
-12,094,882
-47,300
-12,142,182
-29.49
-11,609,292
-11,609,292
-28.20
--1.29
-shareholders holding
-nominal share capital
-in excess of Rs.1 lakhs
-c) Others (specify)
-i) Directors other than
-0.00
-0.00
-0.00
-Promoters
-ii) Trust
-676,142
-676,142
-1.64
-676,142
-676,142
-1.64
-0.00
-iii) Clearing Member
-56,311
-56,311
-0.14
-21,354
-21,354
-0.05
--0.08
-iv) Hindu Undivided
-0.00
-0.00
-0.00
-Families
-Category of
-No. of Shares held at the beginning
-No. of Shares held at the end
-%change
-Shareholders
-of the year
-of the year
-during
-Demat
-Physical
-Total
-% of
-Demat
-Physical
-Total
-% of
-the year
-Total
-Total
-Shares
-Share
-v) NRI
-78,891
-272,705
-351,596
-0.85
-81,289
-271,705
-352,994
-0.86
-0.00
-SUB TOTAL (B)(2):
-18,110,345
-2,076,145
-20,186,490
-49.03
-20,186,490
-49.03
-0.00
-Total Public
-18,112,345
-2,076,245
-20,188,590
-49.04
-20,188,590
-49.04
-0.00
-Shareholding (B)= (B)(1)
-(B)(2)
-C. Shares held by
-0.00
-0.00
-0.00
-Custodian for GDRs
-&amp; ADRs
-Grand Total (A+B+C)
-39,093,422
-2,076,245
-41,169,667
-100.00
-41,169,667
-100.00
-0.00
-Category of
-No. of Shares held at the beginning
-No. of Shares held at the end
-%change
-Shareholders
-of the year
-of the year
-during
-Demat
-Physical
-Total
-% of
-Demat
-Physical
-Total
-% of
-the year
-Total
-Total
-Shares
-Share
-ii)
-Shareholding of Promoters
-Spentex Industries
-20,981,077
-50.96
-20.00
-20,981,077
-50.96
-20.00
-0.00
-Limited
-Sr
-Shareholders
-Shareholding at the
-Shareholding at the
-% change
-No.
-Name
-beginning of the year
-end of the year
-in share
-holding
-No. of
-% of total
-% of shares
-No. of
-% of total
-% of s</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>5666</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.7572338808674811</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>risk management</t>
-        </is>
-      </c>
-      <c r="I9" t="b">
-        <v>0</v>
+The intimation of the Board Meeting of the Company held on 14th December, 2017 for the consideration and approval
+of unaudited Financial Results of the Company for the quarter ended on 30th September,</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>12828</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>0.7833737788563251</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>['risk management']</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+    <row r="12">
+      <c r="A12" t="inlineStr">
         <is>
           <t>Amtek</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Bankers
-Corporation Bank
-Andhra Bank
-Indian Overseas Bank
-IDBI Bank
-Registrar &amp; Share Transfer Agent
-Beetal Financial &amp; Computer
-Services Pvt. Ltd.</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>AMTEK AUTO LIMITED</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
         <is>
           <t>5200770316.pdf</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>2015-16</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
         <is>
           <t>62 | AMTEK AUTO LIMITED
 AUDITORS’ REPORT ON COMPLIANCE OF CONDITIONS OF CORPORATE GOVERNANCE
@@ -5881,50 +6772,59 @@
 from various departments of the Company and the Board is informed of the same at every Board Meeting.</t>
         </is>
       </c>
-      <c r="F10" t="n">
-        <v>4742</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.8014434484576852</v>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>risk management, global economy</t>
-        </is>
-      </c>
-      <c r="I10" t="b">
-        <v>0</v>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>4742</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>0.8014434484576852</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>['risk management', 'global economy']</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+    <row r="13">
+      <c r="A13" t="inlineStr">
         <is>
           <t>Amtek</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Bankers
-Corporation Bank
-Andhra Bank
-Indian Overseas Bank
-IDBI Bank
-Registrar &amp; Share Transfer Agent
-Beetal Financial &amp; Computer
-Services Pvt. Ltd.</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>AMTEK AUTO LIMITED</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
         <is>
           <t>5200770317.pdf</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>2016-17</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
         <is>
           <t>ANNUAL REPORT 2016-17 | 63
 CEO/CFO CERTIFICATE
@@ -6356,46 +7256,59 @@
 systems and processes.</t>
         </is>
       </c>
-      <c r="F11" t="n">
-        <v>4994</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.802535717664869</v>
-      </c>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="b">
-        <v>0</v>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>4994</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>0.802535717664869</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+    <row r="14">
+      <c r="A14" t="inlineStr">
         <is>
           <t>Amtek</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Bankers
-Corporation Bank
-Andhra Bank
-Indian Overseas Bank
-IDBI Bank
-Registrar &amp; Share Transfer Agent
-Beetal Financial &amp; Computer
-Services Pvt. Ltd.</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>AMTEK AUTO LIMITED</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
         <is>
           <t>5200770318.pdf</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>2017-18</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
         <is>
           <t>64 | AMTEK AUTO LIMITED
 (Company under Corporate Insolvency Resolution Process)
@@ -6744,50 +7657,59 @@
 to the Audit Committee and rectify the same.</t>
         </is>
       </c>
-      <c r="F12" t="n">
-        <v>4007</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.7948383526993914</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>global economy</t>
-        </is>
-      </c>
-      <c r="I12" t="b">
-        <v>0</v>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>4007</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>0.7948383526993914</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>['global economy']</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="15">
+      <c r="A15" t="inlineStr">
         <is>
           <t>Amtek</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Bankers
-Corporation Bank
-Andhra Bank
-Indian Overseas Bank
-IDBI Bank
-Registrar &amp; Share Transfer Agent
-Beetal Financial
-&amp; Computer Services Pvt. Ltd.</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>AMTEK AUTO LIMITED</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
         <is>
           <t>5200770915.pdf</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>2014-15</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
         <is>
           <t>56 | AMTEK AUTO LIMITED
 MANAGEMENT DISCUSSION AND ANALYSIS REPORT
@@ -7066,19 +7988,25 @@
 CHAIRMAN</t>
         </is>
       </c>
-      <c r="F13" t="n">
-        <v>3631</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.811975996935779</v>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>risk management, global economy</t>
-        </is>
-      </c>
-      <c r="I13" t="b">
-        <v>0</v>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>3631</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>0.811975996935779</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>['risk management', 'global economy']</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>